<commit_message>
unpool mixed (h x w) and wild (w x w) brood codes
</commit_message>
<xml_diff>
--- a/results/indicators_by_NOAA_pop.xlsx
+++ b/results/indicators_by_NOAA_pop.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa-my.sharepoint.com/personal/thomas_buehrens_dfw_wa_gov/Documents/Documents/Scripts/R5hatchery_indicators_new/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:40009_{3528C564-5877-4DB3-ADB1-633611D56B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5071938-E487-4F67-9718-1334E75C1171}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:40009_{3528C564-5877-4DB3-ADB1-633611D56B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31408B21-FBE7-4696-B073-964C15917D71}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicators_NOAA_pop_markup" sheetId="1" r:id="rId1"/>
     <sheet name="Field_Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indicators_NOAA_pop_markup!$A$1:$S$936</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -849,10 +852,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1210,19 +1212,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S936"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="99.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
@@ -1233,62 +1235,62 @@
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" t="s">
         <v>90</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" t="s">
         <v>91</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" t="s">
         <v>92</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" t="s">
         <v>93</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3781,10 +3783,10 @@
         <v>9</v>
       </c>
       <c r="D44">
-        <v>3.9615976012680999E-2</v>
+        <v>4.1237113402061903E-2</v>
       </c>
       <c r="E44">
-        <v>0.96038402398731904</v>
+        <v>0.95876288659793796</v>
       </c>
       <c r="F44">
         <v>5927622</v>
@@ -3820,7 +3822,7 @@
         <v>0.112</v>
       </c>
       <c r="Q44">
-        <v>4.2707302415131598E-2</v>
+        <v>4.4377385284459003E-2</v>
       </c>
       <c r="R44">
         <v>593</v>
@@ -3840,10 +3842,10 @@
         <v>9</v>
       </c>
       <c r="D45">
-        <v>0.117270191049501</v>
+        <v>0.132712857635298</v>
       </c>
       <c r="E45">
-        <v>0.88272980895049902</v>
+        <v>0.86728714236470195</v>
       </c>
       <c r="F45">
         <v>6738907</v>
@@ -3879,7 +3881,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="Q45">
-        <v>0.11049984446800599</v>
+        <v>0.123257428100901</v>
       </c>
       <c r="R45">
         <v>428</v>
@@ -3899,10 +3901,10 @@
         <v>9</v>
       </c>
       <c r="D46">
-        <v>4.76385408968358E-2</v>
+        <v>4.9986982556625897E-2</v>
       </c>
       <c r="E46">
-        <v>0.95236145910316405</v>
+        <v>0.95001301744337396</v>
       </c>
       <c r="F46">
         <v>6679346</v>
@@ -3938,7 +3940,7 @@
         <v>3.9E-2</v>
       </c>
       <c r="Q46">
-        <v>4.72305379630623E-2</v>
+        <v>4.9443744992855101E-2</v>
       </c>
       <c r="R46">
         <v>288</v>
@@ -3958,10 +3960,10 @@
         <v>9</v>
       </c>
       <c r="D47">
-        <v>0.13465349895036799</v>
+        <v>0.155391828533155</v>
       </c>
       <c r="E47">
-        <v>0.86534650104963196</v>
+        <v>0.84460817146684497</v>
       </c>
       <c r="F47">
         <v>7064595</v>
@@ -3997,7 +3999,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="Q47">
-        <v>0.12964236782184299</v>
+        <v>0.14668022194235</v>
       </c>
       <c r="R47">
         <v>812</v>
@@ -4017,10 +4019,10 @@
         <v>9</v>
       </c>
       <c r="D48">
-        <v>7.5618945584108394E-2</v>
+        <v>8.1743002544529306E-2</v>
       </c>
       <c r="E48">
-        <v>0.92438105441589202</v>
+        <v>0.91825699745547096</v>
       </c>
       <c r="F48">
         <v>7127073</v>
@@ -4056,7 +4058,7 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="Q48">
-        <v>7.6028056694315005E-2</v>
+        <v>8.1682312378588903E-2</v>
       </c>
       <c r="R48">
         <v>764</v>
@@ -4076,10 +4078,10 @@
         <v>9</v>
       </c>
       <c r="D49">
-        <v>9.1813066571872201E-2</v>
+        <v>0.100963031997515</v>
       </c>
       <c r="E49">
-        <v>0.90818693342812795</v>
+        <v>0.899036968002485</v>
       </c>
       <c r="F49">
         <v>4484851</v>
@@ -4115,7 +4117,7 @@
         <v>0.45100000000000001</v>
       </c>
       <c r="Q49">
-        <v>0.143275896452986</v>
+        <v>0.155336576123765</v>
       </c>
       <c r="R49">
         <v>2889</v>
@@ -4607,10 +4609,10 @@
         <v>9</v>
       </c>
       <c r="D58">
-        <v>1.70943774332038E-2</v>
+        <v>1.7391304347826101E-2</v>
       </c>
       <c r="E58">
-        <v>0.98290562256679603</v>
+        <v>0.98260869565217401</v>
       </c>
       <c r="F58">
         <v>559545</v>
@@ -4725,10 +4727,10 @@
         <v>9</v>
       </c>
       <c r="D60">
-        <v>4.0000297289019601E-3</v>
+        <v>4.0160642570281103E-3</v>
       </c>
       <c r="E60">
-        <v>0.99599997027109799</v>
+        <v>0.99598393574297195</v>
       </c>
       <c r="F60">
         <v>268024</v>
@@ -4843,10 +4845,10 @@
         <v>9</v>
       </c>
       <c r="D62">
-        <v>2.6809929056758599E-3</v>
+        <v>2.6881720430107499E-3</v>
       </c>
       <c r="E62">
-        <v>0.99731900709432397</v>
+        <v>0.99731182795698903</v>
       </c>
       <c r="F62">
         <v>481624</v>
@@ -7085,10 +7087,10 @@
         <v>9</v>
       </c>
       <c r="D100">
-        <v>9.8654262966451606E-2</v>
+        <v>0.10934744268077599</v>
       </c>
       <c r="E100">
-        <v>0.90134573703354803</v>
+        <v>0.89065255731922399</v>
       </c>
       <c r="F100">
         <v>4405456</v>
@@ -7124,7 +7126,7 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="Q100">
-        <v>0.23734692930218801</v>
+        <v>0.25647495852965402</v>
       </c>
       <c r="R100">
         <v>2550</v>
@@ -7262,10 +7264,10 @@
         <v>9</v>
       </c>
       <c r="D103">
-        <v>1.0015026621546999E-2</v>
+        <v>1.0116293931333601E-2</v>
       </c>
       <c r="E103">
-        <v>0.98998497337845304</v>
+        <v>0.98988370606866605</v>
       </c>
       <c r="F103">
         <v>3153131</v>
@@ -7301,7 +7303,7 @@
         <v>0.80500000000000005</v>
       </c>
       <c r="Q103">
-        <v>4.8850207648605898E-2</v>
+        <v>4.9319796772070497E-2</v>
       </c>
       <c r="R103">
         <v>3477</v>
@@ -7321,10 +7323,10 @@
         <v>9</v>
       </c>
       <c r="D104">
-        <v>4.4525662045523003E-2</v>
+        <v>4.6599448493266402E-2</v>
       </c>
       <c r="E104">
-        <v>0.955474337954477</v>
+        <v>0.95340055150673397</v>
       </c>
       <c r="F104">
         <v>3447633</v>
@@ -7360,7 +7362,7 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="Q104">
-        <v>0.119523744487922</v>
+        <v>0.124398070207261</v>
       </c>
       <c r="R104">
         <v>2923</v>
@@ -7380,10 +7382,10 @@
         <v>9</v>
       </c>
       <c r="D105">
-        <v>6.7278188927119995E-2</v>
+        <v>7.2125755505784497E-2</v>
       </c>
       <c r="E105">
-        <v>0.93272181107287999</v>
+        <v>0.92787424449421496</v>
       </c>
       <c r="F105">
         <v>3416089</v>
@@ -7419,7 +7421,7 @@
         <v>0.7</v>
       </c>
       <c r="Q105">
-        <v>0.18318046362527199</v>
+        <v>0.19382091789844799</v>
       </c>
       <c r="R105">
         <v>4186</v>
@@ -7439,10 +7441,10 @@
         <v>9</v>
       </c>
       <c r="D106">
-        <v>2.4395142877074599E-2</v>
+        <v>2.5004766957934701E-2</v>
       </c>
       <c r="E106">
-        <v>0.975604857122925</v>
+        <v>0.97499523304206503</v>
       </c>
       <c r="F106">
         <v>2894928</v>
@@ -7478,7 +7480,7 @@
         <v>0.74099999999999999</v>
       </c>
       <c r="Q106">
-        <v>8.6081725429063602E-2</v>
+        <v>8.8043476261925893E-2</v>
       </c>
       <c r="R106">
         <v>2878</v>
@@ -7498,10 +7500,10 @@
         <v>9</v>
       </c>
       <c r="D107">
-        <v>0.176150391495425</v>
+        <v>0.21361632188719401</v>
       </c>
       <c r="E107">
-        <v>0.823849608504575</v>
+        <v>0.78638367811280596</v>
       </c>
       <c r="F107">
         <v>3274631</v>
@@ -7537,7 +7539,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="Q107">
-        <v>0.475888707786501</v>
+        <v>0.52406223798445295</v>
       </c>
       <c r="R107">
         <v>2924</v>
@@ -7557,10 +7559,10 @@
         <v>9</v>
       </c>
       <c r="D108">
-        <v>0.30660935870973999</v>
+        <v>0.44162184137904698</v>
       </c>
       <c r="E108">
-        <v>0.69339064129025996</v>
+        <v>0.55837815862095297</v>
       </c>
       <c r="F108">
         <v>1755813</v>
@@ -7596,7 +7598,7 @@
         <v>0.84499999999999997</v>
       </c>
       <c r="Q108">
-        <v>0.66421824628242798</v>
+        <v>0.74020394620195396</v>
       </c>
       <c r="R108">
         <v>3002</v>
@@ -7616,10 +7618,10 @@
         <v>9</v>
       </c>
       <c r="D109">
-        <v>0.21334046966567699</v>
+        <v>0.271004942339374</v>
       </c>
       <c r="E109">
-        <v>0.78665953033432301</v>
+        <v>0.728995057660626</v>
       </c>
       <c r="F109">
         <v>2311145</v>
@@ -7655,7 +7657,7 @@
         <v>0.89</v>
       </c>
       <c r="Q109">
-        <v>0.65980132300254202</v>
+        <v>0.71128983439270099</v>
       </c>
       <c r="R109">
         <v>4514</v>
@@ -7675,10 +7677,10 @@
         <v>9</v>
       </c>
       <c r="D110">
-        <v>0.19780860785882801</v>
+        <v>0.24594852240228801</v>
       </c>
       <c r="E110">
-        <v>0.80219139214117197</v>
+        <v>0.75405147759771196</v>
       </c>
       <c r="F110">
         <v>3596659</v>
@@ -7714,7 +7716,7 @@
         <v>0.92</v>
       </c>
       <c r="Q110">
-        <v>0.71203196108072697</v>
+        <v>0.754562470753393</v>
       </c>
       <c r="R110">
         <v>4474</v>
@@ -7734,10 +7736,10 @@
         <v>9</v>
       </c>
       <c r="D111">
-        <v>0.156711111939631</v>
+        <v>0.185515873015873</v>
       </c>
       <c r="E111">
-        <v>0.84328888806036895</v>
+        <v>0.81448412698412698</v>
       </c>
       <c r="F111">
         <v>3503839</v>
@@ -7773,7 +7775,7 @@
         <v>0.85</v>
       </c>
       <c r="Q111">
-        <v>0.51094044473509703</v>
+        <v>0.55292726197516295</v>
       </c>
       <c r="R111">
         <v>4043</v>
@@ -7793,10 +7795,10 @@
         <v>9</v>
       </c>
       <c r="D112">
-        <v>0.21975737334284701</v>
+        <v>0.28132678132678102</v>
       </c>
       <c r="E112">
-        <v>0.78024262665715305</v>
+        <v>0.71867321867321898</v>
       </c>
       <c r="F112">
         <v>1187707</v>
@@ -9563,10 +9565,10 @@
         <v>9</v>
       </c>
       <c r="D142">
-        <v>2.46613430153163E-3</v>
+        <v>2.4721878862793601E-3</v>
       </c>
       <c r="E142">
-        <v>0.99753386569846803</v>
+        <v>0.99752781211372099</v>
       </c>
       <c r="F142">
         <v>1256990</v>
@@ -9740,10 +9742,10 @@
         <v>9</v>
       </c>
       <c r="D145">
-        <v>4.2793982791251198E-2</v>
+        <v>4.4705868924313198E-2</v>
       </c>
       <c r="E145">
-        <v>0.95720601720874898</v>
+        <v>0.95529413107568695</v>
       </c>
       <c r="F145">
         <v>1226528</v>
@@ -9779,7 +9781,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="Q145">
-        <v>4.1156213153276701E-2</v>
+        <v>4.2916019058697803E-2</v>
       </c>
       <c r="R145">
         <v>2</v>
@@ -9799,10 +9801,10 @@
         <v>9</v>
       </c>
       <c r="D146">
-        <v>4.2793982791251198E-2</v>
+        <v>4.4705868924313198E-2</v>
       </c>
       <c r="E146">
-        <v>0.95720601720874898</v>
+        <v>0.95529413107568695</v>
       </c>
       <c r="F146">
         <v>1226528</v>
@@ -9858,10 +9860,10 @@
         <v>9</v>
       </c>
       <c r="D147">
-        <v>1.8228092680737201E-2</v>
+        <v>1.85660079601759E-2</v>
       </c>
       <c r="E147">
-        <v>0.981771907319263</v>
+        <v>0.98143399203982395</v>
       </c>
       <c r="F147">
         <v>1292685</v>
@@ -9897,7 +9899,7 @@
         <v>0</v>
       </c>
       <c r="Q147">
-        <v>1.79017774227259E-2</v>
+        <v>1.8227594299319898E-2</v>
       </c>
       <c r="R147">
         <v>0</v>
@@ -9917,10 +9919,10 @@
         <v>9</v>
       </c>
       <c r="D148">
-        <v>1.8228092680737201E-2</v>
+        <v>1.85660079601759E-2</v>
       </c>
       <c r="E148">
-        <v>0.981771907319263</v>
+        <v>0.98143399203982395</v>
       </c>
       <c r="F148">
         <v>1292685</v>
@@ -9976,10 +9978,10 @@
         <v>9</v>
       </c>
       <c r="D149">
-        <v>5.8140210932685298E-4</v>
+        <v>5.8171712924258803E-4</v>
       </c>
       <c r="E149">
-        <v>0.999418597890673</v>
+        <v>0.99941828287075696</v>
       </c>
       <c r="F149">
         <v>601667</v>
@@ -10015,7 +10017,7 @@
         <v>0</v>
       </c>
       <c r="Q149">
-        <v>5.8106427733035796E-4</v>
+        <v>5.8137893115975099E-4</v>
       </c>
       <c r="R149">
         <v>0</v>
@@ -10035,10 +10037,10 @@
         <v>9</v>
       </c>
       <c r="D150">
-        <v>5.8140210932685298E-4</v>
+        <v>5.8171712924258803E-4</v>
       </c>
       <c r="E150">
-        <v>0.999418597890673</v>
+        <v>0.99941828287075696</v>
       </c>
       <c r="F150">
         <v>601667</v>
@@ -10212,10 +10214,10 @@
         <v>9</v>
       </c>
       <c r="D153">
-        <v>5.3662762224331903E-2</v>
+        <v>5.6700273748402703E-2</v>
       </c>
       <c r="E153">
-        <v>0.94633723777566803</v>
+        <v>0.94329972625159697</v>
       </c>
       <c r="F153">
         <v>1304861</v>
@@ -10251,7 +10253,7 @@
         <v>0</v>
       </c>
       <c r="Q153">
-        <v>5.0929732119456603E-2</v>
+        <v>5.3657858483627897E-2</v>
       </c>
       <c r="R153">
         <v>0</v>
@@ -10271,10 +10273,10 @@
         <v>9</v>
       </c>
       <c r="D154">
-        <v>5.3662762224331903E-2</v>
+        <v>5.6700273748402703E-2</v>
       </c>
       <c r="E154">
-        <v>0.94633723777566803</v>
+        <v>0.94329972625159697</v>
       </c>
       <c r="F154">
         <v>1304861</v>
@@ -10448,10 +10450,10 @@
         <v>9</v>
       </c>
       <c r="D157">
-        <v>4.2332036500672297E-3</v>
+        <v>4.25079702444208E-3</v>
       </c>
       <c r="E157">
-        <v>0.99576679634993304</v>
+        <v>0.99574920297555802</v>
       </c>
       <c r="F157">
         <v>1435288</v>
@@ -10487,7 +10489,7 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="Q157">
-        <v>4.8812748776802502E-3</v>
+        <v>4.9014622287193799E-3</v>
       </c>
       <c r="R157">
         <v>29</v>
@@ -10507,10 +10509,10 @@
         <v>9</v>
       </c>
       <c r="D158">
-        <v>6.0503225689929104E-3</v>
+        <v>6.0869565217391303E-3</v>
       </c>
       <c r="E158">
-        <v>0.99394967743100704</v>
+        <v>0.99391304347826104</v>
       </c>
       <c r="F158">
         <v>1745606</v>
@@ -10546,7 +10548,7 @@
         <v>0.47099999999999997</v>
       </c>
       <c r="Q158">
-        <v>1.13079505119123E-2</v>
+        <v>1.13756398797432E-2</v>
       </c>
       <c r="R158">
         <v>165</v>
@@ -10566,10 +10568,10 @@
         <v>9</v>
       </c>
       <c r="D159">
-        <v>4.1633035061102996E-3</v>
+        <v>4.1806020066889604E-3</v>
       </c>
       <c r="E159">
-        <v>0.99583669649388995</v>
+        <v>0.99581939799331098</v>
       </c>
       <c r="F159">
         <v>1562004</v>
@@ -10605,7 +10607,7 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="Q159">
-        <v>5.5646988920732303E-3</v>
+        <v>5.5876909872779401E-3</v>
       </c>
       <c r="R159">
         <v>380</v>
@@ -10625,10 +10627,10 @@
         <v>9</v>
       </c>
       <c r="D160">
-        <v>2.4291796941951199E-3</v>
+        <v>2.4350649350649402E-3</v>
       </c>
       <c r="E160">
-        <v>0.99757082030580502</v>
+        <v>0.99756493506493504</v>
       </c>
       <c r="F160">
         <v>1215829</v>
@@ -11569,10 +11571,10 @@
         <v>9</v>
       </c>
       <c r="D176">
-        <v>0.18410122812881199</v>
+        <v>0.22557471264367801</v>
       </c>
       <c r="E176">
-        <v>0.81589877187118798</v>
+        <v>0.77442528735632199</v>
       </c>
       <c r="F176">
         <v>1573797</v>
@@ -11608,7 +11610,7 @@
         <v>0.11899999999999999</v>
       </c>
       <c r="Q176">
-        <v>0.17284857370059001</v>
+        <v>0.203849509722453</v>
       </c>
       <c r="R176">
         <v>227</v>
@@ -11628,10 +11630,10 @@
         <v>9</v>
       </c>
       <c r="D177">
-        <v>0.174472539957508</v>
+        <v>0.21128798842257601</v>
       </c>
       <c r="E177">
-        <v>0.825527460042492</v>
+        <v>0.78871201157742399</v>
       </c>
       <c r="F177">
         <v>1575534</v>
@@ -11667,7 +11669,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="Q177">
-        <v>0.16736415902582899</v>
+        <v>0.195766089022618</v>
       </c>
       <c r="R177">
         <v>198</v>
@@ -11687,10 +11689,10 @@
         <v>9</v>
       </c>
       <c r="D178">
-        <v>0.18962215619506501</v>
+        <v>0.233918128654971</v>
       </c>
       <c r="E178">
-        <v>0.81037784380493405</v>
+        <v>0.76608187134502903</v>
       </c>
       <c r="F178">
         <v>1514769</v>
@@ -11726,7 +11728,7 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="Q178">
-        <v>0.203758480208932</v>
+        <v>0.23993617697692399</v>
       </c>
       <c r="R178">
         <v>235</v>
@@ -11746,10 +11748,10 @@
         <v>9</v>
       </c>
       <c r="D179">
-        <v>0.25517412429203001</v>
+        <v>0.34248554913294799</v>
       </c>
       <c r="E179">
-        <v>0.74482587570796999</v>
+        <v>0.65751445086705196</v>
       </c>
       <c r="F179">
         <v>1474577</v>
@@ -11785,7 +11787,7 @@
         <v>0.52100000000000002</v>
       </c>
       <c r="Q179">
-        <v>0.34756621876056498</v>
+        <v>0.41691001076577699</v>
       </c>
       <c r="R179">
         <v>914</v>
@@ -11805,10 +11807,10 @@
         <v>9</v>
       </c>
       <c r="D180">
-        <v>0.122596206884871</v>
+        <v>0.13970588235294101</v>
       </c>
       <c r="E180">
-        <v>0.87740379311512895</v>
+        <v>0.86029411764705899</v>
       </c>
       <c r="F180">
         <v>1313349</v>
@@ -11844,7 +11846,7 @@
         <v>0.51400000000000001</v>
       </c>
       <c r="Q180">
-        <v>0.201440964465397</v>
+        <v>0.22327723982325801</v>
       </c>
       <c r="R180">
         <v>403</v>
@@ -11864,10 +11866,10 @@
         <v>9</v>
       </c>
       <c r="D181">
-        <v>0.135539039379869</v>
+        <v>0.15676359039190901</v>
       </c>
       <c r="E181">
-        <v>0.864460960620131</v>
+        <v>0.84323640960809099</v>
       </c>
       <c r="F181">
         <v>1459216</v>
@@ -11903,7 +11905,7 @@
         <v>0.63200000000000001</v>
       </c>
       <c r="Q181">
-        <v>0.26917285211250203</v>
+        <v>0.29873183517711899</v>
       </c>
       <c r="R181">
         <v>374</v>
@@ -11923,10 +11925,10 @@
         <v>9</v>
       </c>
       <c r="D182">
-        <v>6.7572438813618393E-2</v>
+        <v>7.2463768115942004E-2</v>
       </c>
       <c r="E182">
-        <v>0.93242756118638204</v>
+        <v>0.92753623188405798</v>
       </c>
       <c r="F182">
         <v>1422786</v>
@@ -11962,7 +11964,7 @@
         <v>0.46100000000000002</v>
       </c>
       <c r="Q182">
-        <v>0.111400443689433</v>
+        <v>0.118508686686734</v>
       </c>
       <c r="R182">
         <v>367</v>
@@ -11982,10 +11984,10 @@
         <v>9</v>
       </c>
       <c r="D183">
-        <v>8.8366439666292498E-2</v>
+        <v>9.6926713947990503E-2</v>
       </c>
       <c r="E183">
-        <v>0.91163356033370702</v>
+        <v>0.90307328605200898</v>
       </c>
       <c r="F183">
         <v>755688</v>
@@ -12021,7 +12023,7 @@
         <v>0.52900000000000003</v>
       </c>
       <c r="Q183">
-        <v>0.15797594099318901</v>
+        <v>0.170667643496106</v>
       </c>
       <c r="R183">
         <v>312</v>
@@ -12041,10 +12043,10 @@
         <v>9</v>
       </c>
       <c r="D184">
-        <v>3.6185579182941803E-2</v>
+        <v>3.7542662116041001E-2</v>
       </c>
       <c r="E184">
-        <v>0.96381442081705804</v>
+        <v>0.96245733788395904</v>
       </c>
       <c r="F184">
         <v>1121212</v>
@@ -12080,7 +12082,7 @@
         <v>0.57099999999999995</v>
       </c>
       <c r="Q184">
-        <v>7.7787405289946099E-2</v>
+        <v>8.0469944475738298E-2</v>
       </c>
       <c r="R184">
         <v>138</v>
@@ -12100,10 +12102,10 @@
         <v>9</v>
       </c>
       <c r="D185">
-        <v>5.7192824629150298E-2</v>
+        <v>6.0658578856152501E-2</v>
       </c>
       <c r="E185">
-        <v>0.94280717537085001</v>
+        <v>0.939341421143847</v>
       </c>
       <c r="F185">
         <v>1150022</v>
@@ -12139,7 +12141,7 @@
         <v>0.25800000000000001</v>
       </c>
       <c r="Q185">
-        <v>7.1563235888272E-2</v>
+        <v>7.5572080650524495E-2</v>
       </c>
       <c r="R185">
         <v>116</v>
@@ -12159,10 +12161,10 @@
         <v>9</v>
       </c>
       <c r="D186">
-        <v>0.113682825680381</v>
+        <v>0.12824956672443699</v>
       </c>
       <c r="E186">
-        <v>0.88631717431961898</v>
+        <v>0.87175043327556301</v>
       </c>
       <c r="F186">
         <v>645524</v>
@@ -12198,7 +12200,7 @@
         <v>0.49199999999999999</v>
       </c>
       <c r="Q186">
-        <v>0.18286306293882901</v>
+        <v>0.201571165517166</v>
       </c>
       <c r="R186">
         <v>346</v>
@@ -12218,10 +12220,10 @@
         <v>9</v>
       </c>
       <c r="D187">
-        <v>0.21404428428342501</v>
+        <v>0.27229299363057302</v>
       </c>
       <c r="E187">
-        <v>0.78595571571657497</v>
+        <v>0.72770700636942698</v>
       </c>
       <c r="F187">
         <v>1074949</v>
@@ -12257,7 +12259,7 @@
         <v>0.67600000000000005</v>
       </c>
       <c r="Q187">
-        <v>0.39781908392260401</v>
+        <v>0.45664295327821602</v>
       </c>
       <c r="R187">
         <v>552</v>
@@ -12277,10 +12279,10 @@
         <v>9</v>
       </c>
       <c r="D188">
-        <v>0.21972561116365399</v>
+        <v>0.28155339805825202</v>
       </c>
       <c r="E188">
-        <v>0.78027438883634603</v>
+        <v>0.71844660194174803</v>
       </c>
       <c r="F188">
         <v>867994</v>
@@ -14754,14 +14756,14 @@
       <c r="C230" t="s">
         <v>9</v>
       </c>
-      <c r="D230" t="s">
-        <v>10</v>
-      </c>
-      <c r="E230" t="s">
-        <v>10</v>
+      <c r="D230">
+        <v>2.2488755622188899E-3</v>
+      </c>
+      <c r="E230">
+        <v>0.99775112443778102</v>
       </c>
       <c r="F230">
-        <v>0</v>
+        <v>407392</v>
       </c>
       <c r="G230" t="s">
         <v>10</v>
@@ -15699,10 +15701,10 @@
         <v>9</v>
       </c>
       <c r="D246">
-        <v>1.9015548150441999E-2</v>
+        <v>1.9383697813121301E-2</v>
       </c>
       <c r="E246">
-        <v>0.98098445184955796</v>
+        <v>0.98061630218687901</v>
       </c>
       <c r="F246">
         <v>3355864</v>
@@ -15738,7 +15740,7 @@
         <v>0.107</v>
       </c>
       <c r="Q246">
-        <v>2.0850026284097101E-2</v>
+        <v>2.1245116346973101E-2</v>
       </c>
       <c r="R246">
         <v>589</v>
@@ -15935,10 +15937,10 @@
         <v>9</v>
       </c>
       <c r="D250">
-        <v>0.25869547720667901</v>
+        <v>0.34888053124019103</v>
       </c>
       <c r="E250">
-        <v>0.74130452279332104</v>
+        <v>0.65111946875980897</v>
       </c>
       <c r="F250">
         <v>910456</v>
@@ -15974,7 +15976,7 @@
         <v>0.65300000000000002</v>
       </c>
       <c r="Q250">
-        <v>0.42710485209452098</v>
+        <v>0.50135118828287994</v>
       </c>
       <c r="R250">
         <v>997</v>
@@ -15994,10 +15996,10 @@
         <v>9</v>
       </c>
       <c r="D251">
-        <v>0.25617448172149698</v>
+        <v>0.34427950436433202</v>
       </c>
       <c r="E251">
-        <v>0.74382551827850296</v>
+        <v>0.65572049563566803</v>
       </c>
       <c r="F251">
         <v>910456</v>
@@ -16033,7 +16035,7 @@
         <v>0.45600000000000002</v>
       </c>
       <c r="Q251">
-        <v>0.32014827712371302</v>
+        <v>0.38758015092412201</v>
       </c>
       <c r="R251">
         <v>1332</v>
@@ -16053,10 +16055,10 @@
         <v>9</v>
       </c>
       <c r="D252">
-        <v>6.3767907867795501E-2</v>
+        <v>6.81003584229391E-2</v>
       </c>
       <c r="E252">
-        <v>0.93623209213220404</v>
+        <v>0.93189964157706096</v>
       </c>
       <c r="F252">
         <v>1906735</v>
@@ -16092,7 +16094,7 @@
         <v>0.4</v>
       </c>
       <c r="Q252">
-        <v>9.6069585636695695E-2</v>
+        <v>0.101931330472103</v>
       </c>
       <c r="R252">
         <v>883</v>
@@ -16112,10 +16114,10 @@
         <v>9</v>
       </c>
       <c r="D253">
-        <v>4.8041260471536298E-2</v>
+        <v>5.0462573591253203E-2</v>
       </c>
       <c r="E253">
-        <v>0.95195873952846399</v>
+        <v>0.94953742640874705</v>
       </c>
       <c r="F253">
         <v>1939414</v>
@@ -16151,7 +16153,7 @@
         <v>0.59199999999999997</v>
       </c>
       <c r="Q253">
-        <v>0.105344109482249</v>
+        <v>0.11006912340950099</v>
       </c>
       <c r="R253">
         <v>655</v>
@@ -16171,10 +16173,10 @@
         <v>9</v>
       </c>
       <c r="D254">
-        <v>2.4931484122015998E-2</v>
+        <v>2.5568181818181799E-2</v>
       </c>
       <c r="E254">
-        <v>0.97506851587798404</v>
+        <v>0.97443181818181801</v>
       </c>
       <c r="F254">
         <v>1188750</v>
@@ -16210,7 +16212,7 @@
         <v>0.88600000000000001</v>
       </c>
       <c r="Q254">
-        <v>0.17945165042734301</v>
+        <v>0.18319491939423499</v>
       </c>
       <c r="R254">
         <v>903</v>
@@ -16230,10 +16232,10 @@
         <v>9</v>
       </c>
       <c r="D255">
-        <v>3.4707960150243002E-2</v>
+        <v>3.5953686776355902E-2</v>
       </c>
       <c r="E255">
-        <v>0.96529203984975698</v>
+        <v>0.96404631322364398</v>
       </c>
       <c r="F255">
         <v>1902688</v>
@@ -16269,7 +16271,7 @@
         <v>0.86699999999999999</v>
       </c>
       <c r="Q255">
-        <v>0.20695475706191599</v>
+        <v>0.212802025586738</v>
       </c>
       <c r="R255">
         <v>1575</v>
@@ -16289,10 +16291,10 @@
         <v>9</v>
       </c>
       <c r="D256">
-        <v>8.1451894465146293E-2</v>
+        <v>8.8661551577152595E-2</v>
       </c>
       <c r="E256">
-        <v>0.918548105534854</v>
+        <v>0.91133844842284695</v>
       </c>
       <c r="F256">
         <v>2118768</v>
@@ -16328,7 +16330,7 @@
         <v>0.748</v>
       </c>
       <c r="Q256">
-        <v>0.24426880103888601</v>
+        <v>0.26026286549414901</v>
       </c>
       <c r="R256">
         <v>3772</v>
@@ -16348,10 +16350,10 @@
         <v>9</v>
       </c>
       <c r="D257">
-        <v>5.59327017709026E-2</v>
+        <v>5.92417061611374E-2</v>
       </c>
       <c r="E257">
-        <v>0.94406729822909696</v>
+        <v>0.940758293838863</v>
       </c>
       <c r="F257">
         <v>1230834</v>
@@ -16387,7 +16389,7 @@
         <v>0.74299999999999999</v>
       </c>
       <c r="Q257">
-        <v>0.178737158035502</v>
+        <v>0.18733046592833499</v>
       </c>
       <c r="R257">
         <v>1452</v>
@@ -16407,10 +16409,10 @@
         <v>9</v>
       </c>
       <c r="D258">
-        <v>1.39695960240217E-2</v>
+        <v>1.41672000899002E-2</v>
       </c>
       <c r="E258">
-        <v>0.98603040397597796</v>
+        <v>0.98583279991009998</v>
       </c>
       <c r="F258">
         <v>1186974</v>
@@ -19003,10 +19005,10 @@
         <v>35</v>
       </c>
       <c r="D302">
-        <v>0.50028716483261404</v>
+        <v>1</v>
       </c>
       <c r="E302">
-        <v>0.49971283516738602</v>
+        <v>0</v>
       </c>
       <c r="F302">
         <v>250000</v>
@@ -19042,7 +19044,7 @@
         <v>0.95299999999999996</v>
       </c>
       <c r="Q302">
-        <v>0.91412186687335395</v>
+        <v>0.95510983763132795</v>
       </c>
       <c r="R302">
         <v>6082</v>
@@ -19062,10 +19064,10 @@
         <v>35</v>
       </c>
       <c r="D303">
-        <v>0.50071217800074896</v>
+        <v>1</v>
       </c>
       <c r="E303">
-        <v>0.49928782199925098</v>
+        <v>0</v>
       </c>
       <c r="F303">
         <v>206000</v>
@@ -19101,7 +19103,7 @@
         <v>0.93</v>
       </c>
       <c r="Q303">
-        <v>0.87734623037970605</v>
+        <v>0.934579439252336</v>
       </c>
       <c r="R303">
         <v>10052</v>
@@ -19121,10 +19123,10 @@
         <v>35</v>
       </c>
       <c r="D304">
-        <v>0.50071712338329899</v>
+        <v>1</v>
       </c>
       <c r="E304">
-        <v>0.49928287661670101</v>
+        <v>0</v>
       </c>
       <c r="F304">
         <v>157800</v>
@@ -19160,7 +19162,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="Q304">
-        <v>0.947041624411886</v>
+        <v>0.97276264591439698</v>
       </c>
       <c r="R304">
         <v>7782</v>
@@ -19180,10 +19182,10 @@
         <v>35</v>
       </c>
       <c r="D305">
-        <v>0.50081284157519401</v>
+        <v>1</v>
       </c>
       <c r="E305">
-        <v>0.49918715842480599</v>
+        <v>0</v>
       </c>
       <c r="F305">
         <v>151567</v>
@@ -19219,7 +19221,7 @@
         <v>0.94099999999999995</v>
       </c>
       <c r="Q305">
-        <v>0.89460763380492203</v>
+        <v>0.944287063267233</v>
       </c>
       <c r="R305">
         <v>4832</v>
@@ -19239,10 +19241,10 @@
         <v>35</v>
       </c>
       <c r="D306">
-        <v>0.50064092543379701</v>
+        <v>1</v>
       </c>
       <c r="E306">
-        <v>0.49935907456620299</v>
+        <v>0</v>
       </c>
       <c r="F306">
         <v>192156</v>
@@ -19278,7 +19280,7 @@
         <v>0.89</v>
       </c>
       <c r="Q306">
-        <v>0.81986140230962001</v>
+        <v>0.90090090090090102</v>
       </c>
       <c r="R306">
         <v>4267</v>
@@ -19298,10 +19300,10 @@
         <v>35</v>
       </c>
       <c r="D307">
-        <v>0.50044989514254901</v>
+        <v>1</v>
       </c>
       <c r="E307">
-        <v>0.49955010485745099</v>
+        <v>0</v>
       </c>
       <c r="F307">
         <v>141271</v>
@@ -19337,7 +19339,7 @@
         <v>0.93799999999999994</v>
       </c>
       <c r="Q307">
-        <v>0.88976795882540505</v>
+        <v>0.94161958568738202</v>
       </c>
       <c r="R307">
         <v>10857</v>
@@ -19357,10 +19359,10 @@
         <v>35</v>
       </c>
       <c r="D308">
-        <v>0.500480084129028</v>
+        <v>1</v>
       </c>
       <c r="E308">
-        <v>0.499519915870972</v>
+        <v>0</v>
       </c>
       <c r="F308">
         <v>131353</v>
@@ -19396,7 +19398,7 @@
         <v>0.97699999999999998</v>
       </c>
       <c r="Q308">
-        <v>0.95606327595391205</v>
+        <v>0.97751710654936497</v>
       </c>
       <c r="R308">
         <v>30408</v>
@@ -19416,10 +19418,10 @@
         <v>35</v>
       </c>
       <c r="D309">
-        <v>0.50043983377316703</v>
+        <v>1</v>
       </c>
       <c r="E309">
-        <v>0.49956016622683302</v>
+        <v>0</v>
       </c>
       <c r="F309">
         <v>131984</v>
@@ -19455,7 +19457,7 @@
         <v>0.93300000000000005</v>
       </c>
       <c r="Q309">
-        <v>0.88192580779095797</v>
+        <v>0.93720712277413298</v>
       </c>
       <c r="R309">
         <v>6217</v>
@@ -19475,10 +19477,10 @@
         <v>35</v>
       </c>
       <c r="D310">
-        <v>0.50069148965832599</v>
+        <v>1</v>
       </c>
       <c r="E310">
-        <v>0.49930851034167401</v>
+        <v>0</v>
       </c>
       <c r="F310">
         <v>179571</v>
@@ -19514,7 +19516,7 @@
         <v>0.92800000000000005</v>
       </c>
       <c r="Q310">
-        <v>0.87427785937074798</v>
+        <v>0.93283582089552197</v>
       </c>
       <c r="R310">
         <v>6320</v>
@@ -19534,10 +19536,10 @@
         <v>35</v>
       </c>
       <c r="D311">
-        <v>0.50066590855538795</v>
+        <v>1</v>
       </c>
       <c r="E311">
-        <v>0.49933409144461199</v>
+        <v>0</v>
       </c>
       <c r="F311">
         <v>195482</v>
@@ -19573,7 +19575,7 @@
         <v>0.93799999999999994</v>
       </c>
       <c r="Q311">
-        <v>0.88981027807570301</v>
+        <v>0.94161958568738202</v>
       </c>
       <c r="R311">
         <v>7002</v>
@@ -19593,10 +19595,10 @@
         <v>35</v>
       </c>
       <c r="D312">
-        <v>0.50079511260079501</v>
+        <v>1</v>
       </c>
       <c r="E312">
-        <v>0.49920488739920499</v>
+        <v>0</v>
       </c>
       <c r="F312">
         <v>187063</v>
@@ -19632,7 +19634,7 @@
         <v>0.94599999999999995</v>
       </c>
       <c r="Q312">
-        <v>0.90266677053650302</v>
+        <v>0.94876660341555996</v>
       </c>
       <c r="R312">
         <v>12726</v>
@@ -19652,10 +19654,10 @@
         <v>35</v>
       </c>
       <c r="D313">
-        <v>0.50057702710825303</v>
+        <v>1</v>
       </c>
       <c r="E313">
-        <v>0.49942297289174697</v>
+        <v>0</v>
       </c>
       <c r="F313">
         <v>166562</v>
@@ -19711,10 +19713,10 @@
         <v>35</v>
       </c>
       <c r="D314">
-        <v>0.50032006724645195</v>
+        <v>1</v>
       </c>
       <c r="E314">
-        <v>0.499679932753548</v>
+        <v>0</v>
       </c>
       <c r="F314">
         <v>154754</v>
@@ -20773,10 +20775,10 @@
         <v>35</v>
       </c>
       <c r="D332">
-        <v>0.50021990910423697</v>
+        <v>1</v>
       </c>
       <c r="E332">
-        <v>0.49978009089576297</v>
+        <v>0</v>
       </c>
       <c r="F332">
         <v>58004</v>
@@ -20832,10 +20834,10 @@
         <v>35</v>
       </c>
       <c r="D333">
-        <v>0.50025510481008295</v>
+        <v>1</v>
       </c>
       <c r="E333">
-        <v>0.49974489518991699</v>
+        <v>0</v>
       </c>
       <c r="F333">
         <v>46083</v>
@@ -20891,10 +20893,10 @@
         <v>35</v>
       </c>
       <c r="D334">
-        <v>0.50044534007281305</v>
+        <v>1</v>
       </c>
       <c r="E334">
-        <v>0.49955465992718701</v>
+        <v>0</v>
       </c>
       <c r="F334">
         <v>89899</v>
@@ -20930,7 +20932,7 @@
         <v>0.98099999999999998</v>
       </c>
       <c r="Q334">
-        <v>0.96342252296009301</v>
+        <v>0.98135426889107003</v>
       </c>
       <c r="R334">
         <v>2342</v>
@@ -20950,10 +20952,10 @@
         <v>35</v>
       </c>
       <c r="D335">
-        <v>0.50022795163342704</v>
+        <v>1</v>
       </c>
       <c r="E335">
-        <v>0.49977204836657302</v>
+        <v>0</v>
       </c>
       <c r="F335">
         <v>73514</v>
@@ -21009,10 +21011,10 @@
         <v>35</v>
       </c>
       <c r="D336">
-        <v>0.50042939955628696</v>
+        <v>1</v>
       </c>
       <c r="E336">
-        <v>0.49957060044371299</v>
+        <v>0</v>
       </c>
       <c r="F336">
         <v>111880</v>
@@ -21127,10 +21129,10 @@
         <v>35</v>
       </c>
       <c r="D338">
-        <v>0.50022769534362999</v>
+        <v>1</v>
       </c>
       <c r="E338">
-        <v>0.49977230465637001</v>
+        <v>0</v>
       </c>
       <c r="F338">
         <v>105452</v>
@@ -21166,7 +21168,7 @@
         <v>0.98699999999999999</v>
       </c>
       <c r="Q338">
-        <v>0.97467011208096299</v>
+        <v>0.98716683119447202</v>
       </c>
       <c r="R338">
         <v>4855</v>
@@ -21186,10 +21188,10 @@
         <v>35</v>
       </c>
       <c r="D339">
-        <v>0.50021734602392598</v>
+        <v>1</v>
       </c>
       <c r="E339">
-        <v>0.49978265397607402</v>
+        <v>0</v>
       </c>
       <c r="F339">
         <v>110471</v>
@@ -21245,10 +21247,10 @@
         <v>35</v>
       </c>
       <c r="D340">
-        <v>0.50021316590120701</v>
+        <v>1</v>
       </c>
       <c r="E340">
-        <v>0.49978683409879299</v>
+        <v>0</v>
       </c>
       <c r="F340">
         <v>103250</v>
@@ -21304,10 +21306,10 @@
         <v>35</v>
       </c>
       <c r="D341">
-        <v>0.50023400869661405</v>
+        <v>1</v>
       </c>
       <c r="E341">
-        <v>0.499765991303386</v>
+        <v>0</v>
       </c>
       <c r="F341">
         <v>117572</v>
@@ -21363,10 +21365,10 @@
         <v>35</v>
       </c>
       <c r="D342">
-        <v>0.50022346844306298</v>
+        <v>1</v>
       </c>
       <c r="E342">
-        <v>0.49977653155693702</v>
+        <v>0</v>
       </c>
       <c r="F342">
         <v>94015</v>
@@ -26201,10 +26203,10 @@
         <v>43</v>
       </c>
       <c r="D424">
-        <v>0.326492361587777</v>
+        <v>0.48444444444444401</v>
       </c>
       <c r="E424">
-        <v>0.67350763841222205</v>
+        <v>0.51555555555555599</v>
       </c>
       <c r="F424">
         <v>165272</v>
@@ -26240,7 +26242,7 @@
         <v>0.79300000000000004</v>
       </c>
       <c r="Q424">
-        <v>0.61199069582940702</v>
+        <v>0.70062670737586397</v>
       </c>
       <c r="R424">
         <v>1725</v>
@@ -26260,10 +26262,10 @@
         <v>43</v>
       </c>
       <c r="D425">
-        <v>0.21882838762520701</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E425">
-        <v>0.78117161237479305</v>
+        <v>0.72</v>
       </c>
       <c r="F425">
         <v>229000</v>
@@ -26299,7 +26301,7 @@
         <v>0.54100000000000004</v>
       </c>
       <c r="Q425">
-        <v>0.32283744915417201</v>
+        <v>0.37889039242219202</v>
       </c>
       <c r="R425">
         <v>1450</v>
@@ -26437,10 +26439,10 @@
         <v>43</v>
       </c>
       <c r="D428">
-        <v>3.82608469825821E-2</v>
+        <v>3.9776739356178599E-2</v>
       </c>
       <c r="E428">
-        <v>0.96173915301741797</v>
+        <v>0.96022326064382102</v>
       </c>
       <c r="F428">
         <v>963000</v>
@@ -26476,7 +26478,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="Q428">
-        <v>4.5807063890042403E-2</v>
+        <v>4.7535665710286203E-2</v>
       </c>
       <c r="R428">
         <v>479</v>
@@ -26555,10 +26557,10 @@
         <v>43</v>
       </c>
       <c r="D430">
-        <v>7.2283140354370101E-4</v>
+        <v>7.2335262273660601E-4</v>
       </c>
       <c r="E430">
-        <v>0.99927716859645599</v>
+        <v>0.99927664737726296</v>
       </c>
       <c r="F430">
         <v>880000</v>
@@ -26594,7 +26596,7 @@
         <v>0.57499999999999996</v>
       </c>
       <c r="Q430">
-        <v>1.6978920326181099E-3</v>
+        <v>1.69911426817504E-3</v>
       </c>
       <c r="R430">
         <v>461</v>
@@ -26614,10 +26616,10 @@
         <v>43</v>
       </c>
       <c r="D431">
-        <v>1.7218290248823102E-2</v>
+        <v>1.7518713170887101E-2</v>
       </c>
       <c r="E431">
-        <v>0.98278170975117696</v>
+        <v>0.98248128682911295</v>
       </c>
       <c r="F431">
         <v>819000</v>
@@ -26653,7 +26655,7 @@
         <v>0.35599999999999998</v>
       </c>
       <c r="Q431">
-        <v>2.6040251007490502E-2</v>
+        <v>2.6482566285863401E-2</v>
       </c>
       <c r="R431">
         <v>862</v>
@@ -26673,10 +26675,10 @@
         <v>43</v>
       </c>
       <c r="D432">
-        <v>0.113058224985868</v>
+        <v>0.12745098039215699</v>
       </c>
       <c r="E432">
-        <v>0.88694177501413196</v>
+        <v>0.87254901960784303</v>
       </c>
       <c r="F432">
         <v>1076000</v>
@@ -26712,7 +26714,7 @@
         <v>0.59699999999999998</v>
       </c>
       <c r="Q432">
-        <v>0.21908036634618899</v>
+        <v>0.240269101393561</v>
       </c>
       <c r="R432">
         <v>2689</v>
@@ -26732,10 +26734,10 @@
         <v>43</v>
       </c>
       <c r="D433">
-        <v>1.3533409971253201E-2</v>
+        <v>1.37183052843135E-2</v>
       </c>
       <c r="E433">
-        <v>0.98646659002874704</v>
+        <v>0.98628169471568605</v>
       </c>
       <c r="F433">
         <v>908000</v>
@@ -26771,7 +26773,7 @@
         <v>0.51500000000000001</v>
       </c>
       <c r="Q433">
-        <v>2.7146445354652601E-2</v>
+        <v>2.7507122034537899E-2</v>
       </c>
       <c r="R433">
         <v>312</v>
@@ -26791,10 +26793,10 @@
         <v>43</v>
       </c>
       <c r="D434">
-        <v>1.51794399545629E-2</v>
+        <v>1.54132682550896E-2</v>
       </c>
       <c r="E434">
-        <v>0.98482056004543705</v>
+        <v>0.98458673174490996</v>
       </c>
       <c r="F434">
         <v>778550</v>
@@ -26830,7 +26832,7 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="Q434">
-        <v>2.53760643390149E-2</v>
+        <v>2.5756895899105101E-2</v>
       </c>
       <c r="R434">
         <v>627</v>
@@ -26968,10 +26970,10 @@
         <v>43</v>
       </c>
       <c r="D437">
-        <v>6.3515542959090296E-3</v>
+        <v>6.3920454545454497E-3</v>
       </c>
       <c r="E437">
-        <v>0.99364844570409105</v>
+        <v>0.99360795454545503</v>
       </c>
       <c r="F437">
         <v>176000</v>
@@ -27007,7 +27009,7 @@
         <v>0.41099999999999998</v>
       </c>
       <c r="Q437">
-        <v>1.0668577666553099E-2</v>
+        <v>1.0735859679928199E-2</v>
       </c>
       <c r="R437">
         <v>746</v>
@@ -27263,10 +27265,10 @@
         <v>43</v>
       </c>
       <c r="D442">
-        <v>0.15279468511740599</v>
+        <v>0.18027922238965199</v>
       </c>
       <c r="E442">
-        <v>0.84720531488259399</v>
+        <v>0.81972077761034801</v>
       </c>
       <c r="F442">
         <v>749364</v>
@@ -27302,7 +27304,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="Q442">
-        <v>0.137802504979745</v>
+        <v>0.15865750146387</v>
       </c>
       <c r="R442">
         <v>75</v>
@@ -27322,10 +27324,10 @@
         <v>43</v>
       </c>
       <c r="D443">
-        <v>0.25400151535856402</v>
+        <v>0.340157810712234</v>
       </c>
       <c r="E443">
-        <v>0.74599848464143603</v>
+        <v>0.65984218928776595</v>
       </c>
       <c r="F443">
         <v>826557</v>
@@ -27361,7 +27363,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="Q443">
-        <v>0.219534297913038</v>
+        <v>0.27362399832194301</v>
       </c>
       <c r="R443">
         <v>46</v>
@@ -27381,10 +27383,10 @@
         <v>43</v>
       </c>
       <c r="D444">
-        <v>0.138285302215119</v>
+        <v>0.16039492866100999</v>
       </c>
       <c r="E444">
-        <v>0.86171469778488097</v>
+        <v>0.83960507133898998</v>
       </c>
       <c r="F444">
         <v>718495</v>
@@ -27420,7 +27422,7 @@
         <v>0.153</v>
       </c>
       <c r="Q444">
-        <v>0.140350517666533</v>
+        <v>0.15921752641161399</v>
       </c>
       <c r="R444">
         <v>47</v>
@@ -27440,10 +27442,10 @@
         <v>43</v>
       </c>
       <c r="D445">
-        <v>0.31284529771073699</v>
+        <v>0.453917050691244</v>
       </c>
       <c r="E445">
-        <v>0.68715470228926301</v>
+        <v>0.546082949308756</v>
       </c>
       <c r="F445">
         <v>329906</v>
@@ -27479,7 +27481,7 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="Q445">
-        <v>0.26696808727388899</v>
+        <v>0.34573170517684998</v>
       </c>
       <c r="R445">
         <v>59</v>
@@ -27499,10 +27501,10 @@
         <v>43</v>
       </c>
       <c r="D446">
-        <v>0.39939454531232199</v>
+        <v>0.66382978723404296</v>
       </c>
       <c r="E446">
-        <v>0.60060545468767801</v>
+        <v>0.33617021276595699</v>
       </c>
       <c r="F446">
         <v>89680</v>
@@ -27538,7 +27540,7 @@
         <v>0.1</v>
       </c>
       <c r="Q446">
-        <v>0.30736972596442902</v>
+        <v>0.424489795918367</v>
       </c>
       <c r="R446">
         <v>150</v>
@@ -27558,10 +27560,10 @@
         <v>43</v>
       </c>
       <c r="D447">
-        <v>4.6584697201173801E-2</v>
+        <v>4.8834628190899003E-2</v>
       </c>
       <c r="E447">
-        <v>0.95341530279882603</v>
+        <v>0.95116537180910099</v>
       </c>
       <c r="F447">
         <v>491632</v>
@@ -27597,7 +27599,7 @@
         <v>0.12</v>
       </c>
       <c r="Q447">
-        <v>5.0275703173046901E-2</v>
+        <v>5.2576235541535198E-2</v>
       </c>
       <c r="R447">
         <v>31</v>
@@ -28089,10 +28091,10 @@
         <v>43</v>
       </c>
       <c r="D456">
-        <v>0.36303512878654698</v>
+        <v>0.56907667608924395</v>
       </c>
       <c r="E456">
-        <v>0.63696487121345302</v>
+        <v>0.430923323910756</v>
       </c>
       <c r="F456">
         <v>1879882</v>
@@ -28128,7 +28130,7 @@
         <v>0.86499999999999999</v>
       </c>
       <c r="Q456">
-        <v>0.72893478351833396</v>
+        <v>0.80825951975877097</v>
       </c>
       <c r="R456">
         <v>7002</v>
@@ -28148,10 +28150,10 @@
         <v>43</v>
       </c>
       <c r="D457">
-        <v>0.29571591030189998</v>
+        <v>0.41943183334856099</v>
       </c>
       <c r="E457">
-        <v>0.70428408969809997</v>
+        <v>0.58056816665143895</v>
       </c>
       <c r="F457">
         <v>2375113</v>
@@ -28187,7 +28189,7 @@
         <v>0.88900000000000001</v>
       </c>
       <c r="Q457">
-        <v>0.727082228188206</v>
+        <v>0.79073654139633998</v>
       </c>
       <c r="R457">
         <v>5254</v>
@@ -28207,10 +28209,10 @@
         <v>43</v>
       </c>
       <c r="D458">
-        <v>0.270917972358029</v>
+        <v>0.37130554189251003</v>
       </c>
       <c r="E458">
-        <v>0.72908202764197105</v>
+        <v>0.62869445810749003</v>
       </c>
       <c r="F458">
         <v>2069654</v>
@@ -28246,7 +28248,7 @@
         <v>0.871</v>
       </c>
       <c r="Q458">
-        <v>0.67743385164867698</v>
+        <v>0.742157563332138</v>
       </c>
       <c r="R458">
         <v>4610</v>
@@ -28266,10 +28268,10 @@
         <v>43</v>
       </c>
       <c r="D459">
-        <v>9.1082038266951798E-2</v>
+        <v>0.100177851869185</v>
       </c>
       <c r="E459">
-        <v>0.90891796173304795</v>
+        <v>0.89982214813081496</v>
       </c>
       <c r="F459">
         <v>2261971</v>
@@ -28305,7 +28307,7 @@
         <v>0.84099999999999997</v>
       </c>
       <c r="Q459">
-        <v>0.36420863688629102</v>
+        <v>0.38652165355451701</v>
       </c>
       <c r="R459">
         <v>6424</v>
@@ -28325,10 +28327,10 @@
         <v>43</v>
       </c>
       <c r="D460">
-        <v>0.298532343369945</v>
+        <v>0.42496855054204802</v>
       </c>
       <c r="E460">
-        <v>0.70146765663005495</v>
+        <v>0.57503144945795204</v>
       </c>
       <c r="F460">
         <v>2112914</v>
@@ -28364,7 +28366,7 @@
         <v>0.95299999999999996</v>
       </c>
       <c r="Q460">
-        <v>0.86397800118618895</v>
+        <v>0.90041709358383903</v>
       </c>
       <c r="R460">
         <v>24951</v>
@@ -28384,10 +28386,10 @@
         <v>43</v>
       </c>
       <c r="D461">
-        <v>0.139007297235995</v>
+        <v>0.16132499225125799</v>
       </c>
       <c r="E461">
-        <v>0.86099270276400497</v>
+        <v>0.83867500774874204</v>
       </c>
       <c r="F461">
         <v>2375837</v>
@@ -28423,7 +28425,7 @@
         <v>0.92500000000000004</v>
       </c>
       <c r="Q461">
-        <v>0.64954466053886695</v>
+        <v>0.68264042120326796</v>
       </c>
       <c r="R461">
         <v>2540</v>
@@ -30685,10 +30687,10 @@
         <v>43</v>
       </c>
       <c r="D500">
-        <v>8.7971884033506299E-3</v>
+        <v>8.8747463130704404E-3</v>
       </c>
       <c r="E500">
-        <v>0.99120281159664902</v>
+        <v>0.99112525368693005</v>
       </c>
       <c r="F500">
         <v>2050206</v>
@@ -30724,7 +30726,7 @@
         <v>0.84699999999999998</v>
       </c>
       <c r="Q500">
-        <v>5.4371701326600103E-2</v>
+        <v>5.4824773568487403E-2</v>
       </c>
       <c r="R500">
         <v>1524</v>
@@ -30803,10 +30805,10 @@
         <v>43</v>
       </c>
       <c r="D502">
-        <v>0.129455680667832</v>
+        <v>8.3924530361478594E-2</v>
       </c>
       <c r="E502">
-        <v>0.87054431933216803</v>
+        <v>0.91607546963852104</v>
       </c>
       <c r="F502">
         <v>2177701</v>
@@ -30842,7 +30844,7 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="Q502">
-        <v>0.16502612430267899</v>
+        <v>0.113576592619578</v>
       </c>
       <c r="R502">
         <v>4840</v>
@@ -30862,10 +30864,10 @@
         <v>43</v>
       </c>
       <c r="D503">
-        <v>1.85313725397614E-2</v>
+        <v>1.8879682117354302E-2</v>
       </c>
       <c r="E503">
-        <v>0.981468627460239</v>
+        <v>0.98112031788264598</v>
       </c>
       <c r="F503">
         <v>1666442</v>
@@ -30901,7 +30903,7 @@
         <v>0.21</v>
       </c>
       <c r="Q503">
-        <v>2.2919794047756702E-2</v>
+        <v>2.3340532015755599E-2</v>
       </c>
       <c r="R503">
         <v>1007</v>
@@ -30921,10 +30923,10 @@
         <v>43</v>
       </c>
       <c r="D504">
-        <v>0.12215373424612699</v>
+        <v>0.139061910647126</v>
       </c>
       <c r="E504">
-        <v>0.87784626575387303</v>
+        <v>0.86093808935287397</v>
       </c>
       <c r="F504">
         <v>2016371</v>
@@ -30960,7 +30962,7 @@
         <v>0.34699999999999998</v>
       </c>
       <c r="Q504">
-        <v>0.15758646169063101</v>
+        <v>0.175569496244946</v>
       </c>
       <c r="R504">
         <v>3350</v>
@@ -30980,10 +30982,10 @@
         <v>43</v>
       </c>
       <c r="D505">
-        <v>6.1344912806197201E-2</v>
+        <v>6.53277713855204E-2</v>
       </c>
       <c r="E505">
-        <v>0.93865508719380297</v>
+        <v>0.93467222861447996</v>
       </c>
       <c r="F505">
         <v>2193389</v>
@@ -31019,7 +31021,7 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="Q505">
-        <v>9.9854188628317395E-2</v>
+        <v>0.10565233264412</v>
       </c>
       <c r="R505">
         <v>4274</v>
@@ -31039,10 +31041,10 @@
         <v>43</v>
       </c>
       <c r="D506">
-        <v>1.37815097980995E-2</v>
+        <v>1.3972970828221401E-2</v>
       </c>
       <c r="E506">
-        <v>0.9862184902019</v>
+        <v>0.98602702917177898</v>
       </c>
       <c r="F506">
         <v>1916165</v>
@@ -31078,7 +31080,7 @@
         <v>0.28899999999999998</v>
       </c>
       <c r="Q506">
-        <v>1.90147094148947E-2</v>
+        <v>1.9273781769075401E-2</v>
       </c>
       <c r="R506">
         <v>2984</v>
@@ -31098,10 +31100,10 @@
         <v>43</v>
       </c>
       <c r="D507">
-        <v>3.5654673494957802E-2</v>
+        <v>3.6968115358456899E-2</v>
       </c>
       <c r="E507">
-        <v>0.96434532650504201</v>
+        <v>0.96303188464154299</v>
       </c>
       <c r="F507">
         <v>1957690</v>
@@ -31137,7 +31139,7 @@
         <v>0.47699999999999998</v>
       </c>
       <c r="Q507">
-        <v>6.3822384715590402E-2</v>
+        <v>6.6018250583414498E-2</v>
       </c>
       <c r="R507">
         <v>4433</v>
@@ -31157,10 +31159,10 @@
         <v>43</v>
       </c>
       <c r="D508">
-        <v>0.11158906066161001</v>
+        <v>0.12556763630935999</v>
       </c>
       <c r="E508">
-        <v>0.88841093933838999</v>
+        <v>0.87443236369064004</v>
       </c>
       <c r="F508">
         <v>2155007</v>
@@ -31196,7 +31198,7 @@
         <v>0.56100000000000005</v>
       </c>
       <c r="Q508">
-        <v>0.20267213541714801</v>
+        <v>0.222413805244327</v>
       </c>
       <c r="R508">
         <v>7739</v>
@@ -31216,10 +31218,10 @@
         <v>43</v>
       </c>
       <c r="D509">
-        <v>0.17579059552849599</v>
+        <v>0.21316764906092001</v>
       </c>
       <c r="E509">
-        <v>0.82420940447150404</v>
+        <v>0.78683235093907999</v>
       </c>
       <c r="F509">
         <v>2146597</v>
@@ -31255,7 +31257,7 @@
         <v>0.378</v>
       </c>
       <c r="Q509">
-        <v>0.22034678838504401</v>
+        <v>0.25523935140520598</v>
       </c>
       <c r="R509">
         <v>4761</v>
@@ -31393,10 +31395,10 @@
         <v>43</v>
       </c>
       <c r="D512">
-        <v>0.33348220612296597</v>
+        <v>0.5</v>
       </c>
       <c r="E512">
-        <v>0.66651779387703403</v>
+        <v>0.5</v>
       </c>
       <c r="F512">
         <v>155310</v>
@@ -31432,7 +31434,7 @@
         <v>0.443</v>
       </c>
       <c r="Q512">
-        <v>0.37449620422501301</v>
+        <v>0.47303689687795702</v>
       </c>
       <c r="R512">
         <v>1644</v>
@@ -31452,10 +31454,10 @@
         <v>43</v>
       </c>
       <c r="D513">
-        <v>0.500404518347359</v>
+        <v>1</v>
       </c>
       <c r="E513">
-        <v>0.499595481652641</v>
+        <v>0</v>
       </c>
       <c r="F513">
         <v>163289</v>
@@ -31491,7 +31493,7 @@
         <v>0.77700000000000002</v>
       </c>
       <c r="Q513">
-        <v>0.69173540620198104</v>
+        <v>0.81766148814390804</v>
       </c>
       <c r="R513">
         <v>947</v>
@@ -31511,10 +31513,10 @@
         <v>43</v>
       </c>
       <c r="D514">
-        <v>0.50022030532456296</v>
+        <v>1</v>
       </c>
       <c r="E514">
-        <v>0.49977969467543698</v>
+        <v>0</v>
       </c>
       <c r="F514">
         <v>161211</v>
@@ -31550,7 +31552,7 @@
         <v>0.80200000000000005</v>
       </c>
       <c r="Q514">
-        <v>0.71642188219094904</v>
+        <v>0.83472454090150205</v>
       </c>
       <c r="R514">
         <v>1366</v>
@@ -31570,10 +31572,10 @@
         <v>43</v>
       </c>
       <c r="D515">
-        <v>0.50017689938085197</v>
+        <v>1</v>
       </c>
       <c r="E515">
-        <v>0.49982310061914798</v>
+        <v>0</v>
       </c>
       <c r="F515">
         <v>163993</v>
@@ -31609,7 +31611,7 @@
         <v>0.80100000000000005</v>
       </c>
       <c r="Q515">
-        <v>0.71537961254695004</v>
+        <v>0.83402835696413702</v>
       </c>
       <c r="R515">
         <v>2300</v>
@@ -31629,10 +31631,10 @@
         <v>43</v>
       </c>
       <c r="D516">
-        <v>0.50130491518051301</v>
+        <v>1</v>
       </c>
       <c r="E516">
-        <v>0.49869508481948699</v>
+        <v>0</v>
       </c>
       <c r="F516">
         <v>25355</v>
@@ -31668,7 +31670,7 @@
         <v>0.67600000000000005</v>
       </c>
       <c r="Q516">
-        <v>0.60741782335182903</v>
+        <v>0.75528700906344404</v>
       </c>
       <c r="R516">
         <v>4567</v>
@@ -31688,10 +31690,10 @@
         <v>43</v>
       </c>
       <c r="D517">
-        <v>0.21050918192540299</v>
+        <v>0.26245591535748602</v>
       </c>
       <c r="E517">
-        <v>0.78949081807459698</v>
+        <v>0.73754408464251398</v>
       </c>
       <c r="F517">
         <v>124760</v>
@@ -31727,7 +31729,7 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="Q517">
-        <v>0.27643682692459498</v>
+        <v>0.322643071864744</v>
       </c>
       <c r="R517">
         <v>830</v>
@@ -31747,10 +31749,10 @@
         <v>43</v>
       </c>
       <c r="D518">
-        <v>0.40099549396073197</v>
+        <v>0.66901408450704203</v>
       </c>
       <c r="E518">
-        <v>0.59900450603926803</v>
+        <v>0.33098591549295803</v>
       </c>
       <c r="F518">
         <v>150546</v>
@@ -31786,7 +31788,7 @@
         <v>0.38600000000000001</v>
       </c>
       <c r="Q518">
-        <v>0.39507120607596102</v>
+        <v>0.52143939227611003</v>
       </c>
       <c r="R518">
         <v>1818</v>
@@ -31806,10 +31808,10 @@
         <v>43</v>
       </c>
       <c r="D519">
-        <v>0.416159855678432</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="E519">
-        <v>0.58384014432156806</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="F519">
         <v>79537</v>
@@ -31845,7 +31847,7 @@
         <v>0.75800000000000001</v>
       </c>
       <c r="Q519">
-        <v>0.63230817268466499</v>
+        <v>0.74633123689727499</v>
       </c>
       <c r="R519">
         <v>889</v>
@@ -31865,10 +31867,10 @@
         <v>43</v>
       </c>
       <c r="D520">
-        <v>7.1902130537440601E-2</v>
+        <v>7.7464788732394402E-2</v>
       </c>
       <c r="E520">
-        <v>0.92809786946255901</v>
+        <v>0.92253521126760596</v>
       </c>
       <c r="F520">
         <v>109468</v>
@@ -31904,7 +31906,7 @@
         <v>0.75</v>
       </c>
       <c r="Q520">
-        <v>0.22336643257810801</v>
+        <v>0.236559139784946</v>
       </c>
       <c r="R520">
         <v>913</v>
@@ -31924,10 +31926,10 @@
         <v>43</v>
       </c>
       <c r="D521">
-        <v>0.35939912816612701</v>
+        <v>0.56050955414012704</v>
       </c>
       <c r="E521">
-        <v>0.64060087183387304</v>
+        <v>0.43949044585987301</v>
       </c>
       <c r="F521">
         <v>94067</v>
@@ -31963,7 +31965,7 @@
         <v>0.8</v>
       </c>
       <c r="Q521">
-        <v>0.64247352216000397</v>
+        <v>0.73701842546063601</v>
       </c>
       <c r="R521">
         <v>2087</v>
@@ -31983,10 +31985,10 @@
         <v>43</v>
       </c>
       <c r="D522">
-        <v>0.39931369795484001</v>
+        <v>0.66412213740458004</v>
       </c>
       <c r="E522">
-        <v>0.60068630204516005</v>
+        <v>0.33587786259542002</v>
       </c>
       <c r="F522">
         <v>90322</v>
@@ -32022,7 +32024,7 @@
         <v>0.84</v>
       </c>
       <c r="Q522">
-        <v>0.71393513052684299</v>
+        <v>0.80585402000741002</v>
       </c>
       <c r="R522">
         <v>2021</v>
@@ -32042,10 +32044,10 @@
         <v>43</v>
       </c>
       <c r="D523">
-        <v>0.42043827731217798</v>
+        <v>0.72463768115941996</v>
       </c>
       <c r="E523">
-        <v>0.57956172268782202</v>
+        <v>0.27536231884057999</v>
       </c>
       <c r="F523">
         <v>90220</v>
@@ -32081,7 +32083,7 @@
         <v>0.85799999999999998</v>
       </c>
       <c r="Q523">
-        <v>0.747527851982976</v>
+        <v>0.83614836616609201</v>
       </c>
       <c r="R523">
         <v>2316</v>
@@ -35051,10 +35053,10 @@
         <v>43</v>
       </c>
       <c r="D574">
-        <v>0.50085648965880403</v>
+        <v>1</v>
       </c>
       <c r="E574">
-        <v>0.49914351034119597</v>
+        <v>0</v>
       </c>
       <c r="F574">
         <v>1127160</v>
@@ -35090,7 +35092,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="Q574">
-        <v>0.355758199317735</v>
+        <v>0.52438384897745105</v>
       </c>
       <c r="R574">
         <v>911</v>
@@ -35110,10 +35112,10 @@
         <v>43</v>
       </c>
       <c r="D575">
-        <v>0.50011750775677699</v>
+        <v>0.99747474747474796</v>
       </c>
       <c r="E575">
-        <v>0.49988249224322301</v>
+        <v>2.5252525252524899E-3</v>
       </c>
       <c r="F575">
         <v>1055449</v>
@@ -35149,7 +35151,7 @@
         <v>0.44600000000000001</v>
       </c>
       <c r="Q575">
-        <v>0.47444189483301102</v>
+        <v>0.64292038855178502</v>
       </c>
       <c r="R575">
         <v>5200</v>
@@ -35169,10 +35171,10 @@
         <v>43</v>
       </c>
       <c r="D576">
-        <v>0.43806913097592698</v>
+        <v>0.77746077032810301</v>
       </c>
       <c r="E576">
-        <v>0.56193086902407297</v>
+        <v>0.22253922967189699</v>
       </c>
       <c r="F576">
         <v>1003205</v>
@@ -35208,7 +35210,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="Q576">
-        <v>0.31089257535045001</v>
+        <v>0.44465439746881502</v>
       </c>
       <c r="R576">
         <v>172</v>
@@ -35228,10 +35230,10 @@
         <v>43</v>
       </c>
       <c r="D577">
-        <v>0.50082562531859598</v>
+        <v>1</v>
       </c>
       <c r="E577">
-        <v>0.49917437468140402</v>
+        <v>0</v>
       </c>
       <c r="F577">
         <v>919608</v>
@@ -35267,7 +35269,7 @@
         <v>0.36599999999999999</v>
       </c>
       <c r="Q577">
-        <v>0.44132385993486201</v>
+        <v>0.61199510403916801</v>
       </c>
       <c r="R577">
         <v>3562</v>
@@ -35287,10 +35289,10 @@
         <v>43</v>
       </c>
       <c r="D578">
-        <v>0.50084941094579105</v>
+        <v>1</v>
       </c>
       <c r="E578">
-        <v>0.499150589054209</v>
+        <v>0</v>
       </c>
       <c r="F578">
         <v>968489</v>
@@ -35326,7 +35328,7 @@
         <v>0.41899999999999998</v>
       </c>
       <c r="Q578">
-        <v>0.46295667944019198</v>
+        <v>0.63251106894370701</v>
       </c>
       <c r="R578">
         <v>8915</v>
@@ -35346,10 +35348,10 @@
         <v>43</v>
       </c>
       <c r="D579">
-        <v>0.50025720138555296</v>
+        <v>0.99730458221024298</v>
       </c>
       <c r="E579">
-        <v>0.49974279861444698</v>
+        <v>2.6954177897574598E-3</v>
       </c>
       <c r="F579">
         <v>994377</v>
@@ -35385,7 +35387,7 @@
         <v>0.32800000000000001</v>
       </c>
       <c r="Q579">
-        <v>0.42674696371604498</v>
+        <v>0.59743715606996195</v>
       </c>
       <c r="R579">
         <v>9666</v>
@@ -36467,10 +36469,10 @@
         <v>43</v>
       </c>
       <c r="D598">
-        <v>0.166145533412625</v>
+        <v>0.19923332085651199</v>
       </c>
       <c r="E598">
-        <v>0.83385446658737505</v>
+        <v>0.80076667914348798</v>
       </c>
       <c r="F598">
         <v>154954</v>
@@ -36506,7 +36508,7 @@
         <v>0.879</v>
       </c>
       <c r="Q598">
-        <v>0.57861089266492405</v>
+        <v>0.62215050052765497</v>
       </c>
       <c r="R598">
         <v>386</v>
@@ -36526,10 +36528,10 @@
         <v>43</v>
       </c>
       <c r="D599">
-        <v>0.49486100770693398</v>
+        <v>0.978494623655914</v>
       </c>
       <c r="E599">
-        <v>0.50513899229306602</v>
+        <v>2.1505376344085999E-2</v>
       </c>
       <c r="F599">
         <v>153899</v>
@@ -36565,7 +36567,7 @@
         <v>0.66400000000000003</v>
       </c>
       <c r="Q599">
-        <v>0.595600230503878</v>
+        <v>0.74438845625286298</v>
       </c>
       <c r="R599">
         <v>423</v>
@@ -36585,10 +36587,10 @@
         <v>43</v>
       </c>
       <c r="D600">
-        <v>0.33350991422076798</v>
+        <v>0.5</v>
       </c>
       <c r="E600">
-        <v>0.66649008577923197</v>
+        <v>0.5</v>
       </c>
       <c r="F600">
         <v>153615</v>
@@ -36624,7 +36626,7 @@
         <v>0.315</v>
       </c>
       <c r="Q600">
-        <v>0.32744886383941302</v>
+        <v>0.42194092827004198</v>
       </c>
       <c r="R600">
         <v>834</v>
@@ -36644,10 +36646,10 @@
         <v>43</v>
       </c>
       <c r="D601">
-        <v>0.33343421149254399</v>
+        <v>0.5</v>
       </c>
       <c r="E601">
-        <v>0.66656578850745596</v>
+        <v>0.5</v>
       </c>
       <c r="F601">
         <v>149841</v>
@@ -36683,7 +36685,7 @@
         <v>0.38200000000000001</v>
       </c>
       <c r="Q601">
-        <v>0.35045430095421498</v>
+        <v>0.44722719141323802</v>
       </c>
       <c r="R601">
         <v>151</v>
@@ -36703,10 +36705,10 @@
         <v>43</v>
       </c>
       <c r="D602">
-        <v>0.333514072923211</v>
+        <v>0.5</v>
       </c>
       <c r="E602">
-        <v>0.666485927076789</v>
+        <v>0.5</v>
       </c>
       <c r="F602">
         <v>127939</v>
@@ -36742,7 +36744,7 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="Q602">
-        <v>0.31597311819780399</v>
+        <v>0.40916530278232399</v>
       </c>
       <c r="R602">
         <v>322</v>
@@ -36762,10 +36764,10 @@
         <v>43</v>
       </c>
       <c r="D603">
-        <v>0.333739899374905</v>
+        <v>0.5</v>
       </c>
       <c r="E603">
-        <v>0.666260100625095</v>
+        <v>0.5</v>
       </c>
       <c r="F603">
         <v>142285</v>
@@ -36801,7 +36803,7 @@
         <v>0.25</v>
       </c>
       <c r="Q603">
-        <v>0.30795202757359402</v>
+        <v>0.4</v>
       </c>
       <c r="R603">
         <v>272</v>
@@ -36821,10 +36823,10 @@
         <v>43</v>
       </c>
       <c r="D604">
-        <v>0.33364589898493002</v>
+        <v>0.5</v>
       </c>
       <c r="E604">
-        <v>0.66635410101506998</v>
+        <v>0.5</v>
       </c>
       <c r="F604">
         <v>130228</v>
@@ -36860,7 +36862,7 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="Q604">
-        <v>0.32185136632637201</v>
+        <v>0.41562759767248603</v>
       </c>
       <c r="R604">
         <v>302</v>
@@ -36880,10 +36882,10 @@
         <v>43</v>
       </c>
       <c r="D605">
-        <v>0.33350748762188298</v>
+        <v>0.5</v>
       </c>
       <c r="E605">
-        <v>0.66649251237811702</v>
+        <v>0.5</v>
       </c>
       <c r="F605">
         <v>109794</v>
@@ -36919,7 +36921,7 @@
         <v>0.45100000000000001</v>
       </c>
       <c r="Q605">
-        <v>0.37790896088665998</v>
+        <v>0.47664442326024797</v>
       </c>
       <c r="R605">
         <v>584</v>
@@ -36939,10 +36941,10 @@
         <v>43</v>
       </c>
       <c r="D606">
-        <v>0.33341551397503399</v>
+        <v>0.5</v>
       </c>
       <c r="E606">
-        <v>0.66658448602496601</v>
+        <v>0.5</v>
       </c>
       <c r="F606">
         <v>102780</v>
@@ -36978,7 +36980,7 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="Q606">
-        <v>0.35416403174324201</v>
+        <v>0.45126353790613699</v>
       </c>
       <c r="R606">
         <v>858</v>
@@ -36998,10 +37000,10 @@
         <v>43</v>
       </c>
       <c r="D607">
-        <v>0.33351190929153002</v>
+        <v>0.5</v>
       </c>
       <c r="E607">
-        <v>0.66648809070847004</v>
+        <v>0.5</v>
       </c>
       <c r="F607">
         <v>109567</v>
@@ -37037,7 +37039,7 @@
         <v>0.82699999999999996</v>
       </c>
       <c r="Q607">
-        <v>0.65844830728268799</v>
+        <v>0.74294205052005902</v>
       </c>
       <c r="R607">
         <v>860</v>
@@ -39771,10 +39773,10 @@
         <v>61</v>
       </c>
       <c r="D654">
-        <v>0.50020723114806098</v>
+        <v>1</v>
       </c>
       <c r="E654">
-        <v>0.49979276885193902</v>
+        <v>0</v>
       </c>
       <c r="F654">
         <v>90385</v>
@@ -39810,7 +39812,7 @@
         <v>0.49405772495755501</v>
       </c>
       <c r="Q654">
-        <v>0.49715000412011401</v>
+        <v>0.66403607666290898</v>
       </c>
       <c r="R654">
         <v>582</v>
@@ -39830,10 +39832,10 @@
         <v>61</v>
       </c>
       <c r="D655">
-        <v>0.50020723114806098</v>
+        <v>1</v>
       </c>
       <c r="E655">
-        <v>0.49979276885193902</v>
+        <v>0</v>
       </c>
       <c r="F655">
         <v>90385</v>
@@ -39869,7 +39871,7 @@
         <v>0.495</v>
       </c>
       <c r="Q655">
-        <v>0.49761602945968397</v>
+        <v>0.66445182724252505</v>
       </c>
       <c r="R655" t="s">
         <v>10</v>
@@ -39889,10 +39891,10 @@
         <v>61</v>
       </c>
       <c r="D656">
-        <v>0.40014785088182497</v>
+        <v>0.66670332449879599</v>
       </c>
       <c r="E656">
-        <v>0.59985214911817497</v>
+        <v>0.33329667550120401</v>
       </c>
       <c r="F656">
         <v>90931</v>
@@ -39928,7 +39930,7 @@
         <v>0.55260977630488795</v>
       </c>
       <c r="Q656">
-        <v>0.47212964571717397</v>
+        <v>0.59842669906814305</v>
       </c>
       <c r="R656">
         <v>667</v>
@@ -39948,10 +39950,10 @@
         <v>61</v>
       </c>
       <c r="D657">
-        <v>0.40014785088182497</v>
+        <v>0.66670332449879599</v>
       </c>
       <c r="E657">
-        <v>0.59985214911817497</v>
+        <v>0.33329667550120401</v>
       </c>
       <c r="F657">
         <v>90931</v>
@@ -39987,7 +39989,7 @@
         <v>0.55200000000000005</v>
       </c>
       <c r="Q657">
-        <v>0.47179020788154902</v>
+        <v>0.59809934163295497</v>
       </c>
       <c r="R657" t="s">
         <v>10</v>
@@ -40007,10 +40009,10 @@
         <v>61</v>
       </c>
       <c r="D658">
-        <v>0.43317102207302999</v>
+        <v>0.76351705811023496</v>
       </c>
       <c r="E658">
-        <v>0.56682897792696996</v>
+        <v>0.23648294188976501</v>
       </c>
       <c r="F658">
         <v>116279</v>
@@ -40046,7 +40048,7 @@
         <v>0.62816188870151801</v>
       </c>
       <c r="Q658">
-        <v>0.53809454342317597</v>
+        <v>0.67249181461680196</v>
       </c>
       <c r="R658">
         <v>745</v>
@@ -40066,10 +40068,10 @@
         <v>61</v>
       </c>
       <c r="D659">
-        <v>0.43317102207302999</v>
+        <v>0.76351705811023496</v>
       </c>
       <c r="E659">
-        <v>0.56682897792696996</v>
+        <v>0.23648294188976501</v>
       </c>
       <c r="F659">
         <v>116279</v>
@@ -40105,7 +40107,7 @@
         <v>0.63</v>
       </c>
       <c r="Q659">
-        <v>0.53932600924145802</v>
+        <v>0.67358232736536605</v>
       </c>
       <c r="R659" t="s">
         <v>10</v>
@@ -40125,10 +40127,10 @@
         <v>61</v>
       </c>
       <c r="D660">
-        <v>0.43184166674424501</v>
+        <v>0.75945056564234403</v>
       </c>
       <c r="E660">
-        <v>0.56815833325575504</v>
+        <v>0.24054943435765599</v>
       </c>
       <c r="F660">
         <v>122162</v>
@@ -40164,7 +40166,7 @@
         <v>0.53528628495339503</v>
       </c>
       <c r="Q660">
-        <v>0.481667586314245</v>
+        <v>0.62038288293702903</v>
       </c>
       <c r="R660">
         <v>402</v>
@@ -40184,10 +40186,10 @@
         <v>61</v>
       </c>
       <c r="D661">
-        <v>0.43184166674424501</v>
+        <v>0.75945056564234403</v>
       </c>
       <c r="E661">
-        <v>0.56815833325575504</v>
+        <v>0.24054943435765599</v>
       </c>
       <c r="F661">
         <v>122162</v>
@@ -40223,7 +40225,7 @@
         <v>0.53700000000000003</v>
       </c>
       <c r="Q661">
-        <v>0.48259002993841299</v>
+        <v>0.62125257821226199</v>
       </c>
       <c r="R661" t="s">
         <v>10</v>
@@ -40243,10 +40245,10 @@
         <v>61</v>
       </c>
       <c r="D662">
-        <v>0.41458623784339099</v>
+        <v>0.7076204238921</v>
       </c>
       <c r="E662">
-        <v>0.58541376215660901</v>
+        <v>0.2923795761079</v>
       </c>
       <c r="F662">
         <v>103800</v>
@@ -40282,7 +40284,7 @@
         <v>0.423097392229909</v>
       </c>
       <c r="Q662">
-        <v>0.41814513564887001</v>
+        <v>0.55088184987732702</v>
       </c>
       <c r="R662">
         <v>795</v>
@@ -40302,10 +40304,10 @@
         <v>61</v>
       </c>
       <c r="D663">
-        <v>0.41458623784339099</v>
+        <v>0.7076204238921</v>
       </c>
       <c r="E663">
-        <v>0.58541376215660901</v>
+        <v>0.2923795761079</v>
       </c>
       <c r="F663">
         <v>103800</v>
@@ -40341,7 +40343,7 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="Q663">
-        <v>0.418526143413811</v>
+        <v>0.55126921535457096</v>
       </c>
       <c r="R663" t="s">
         <v>10</v>
@@ -40361,10 +40363,10 @@
         <v>61</v>
       </c>
       <c r="D664">
-        <v>0.38265090755593101</v>
+        <v>0.619283778514644</v>
       </c>
       <c r="E664">
-        <v>0.61734909244406899</v>
+        <v>0.380716221485356</v>
       </c>
       <c r="F664">
         <v>79570</v>
@@ -40400,7 +40402,7 @@
         <v>0.64700000000000002</v>
       </c>
       <c r="Q664">
-        <v>0.52015283829013503</v>
+        <v>0.63693727304668502</v>
       </c>
       <c r="R664">
         <v>877</v>
@@ -40420,10 +40422,10 @@
         <v>61</v>
       </c>
       <c r="D665">
-        <v>0.37510038727178602</v>
+        <v>0.6</v>
       </c>
       <c r="E665">
-        <v>0.62489961272821404</v>
+        <v>0.4</v>
       </c>
       <c r="F665">
         <v>91078</v>
@@ -40459,7 +40461,7 @@
         <v>0.54300000000000004</v>
       </c>
       <c r="Q665">
-        <v>0.450787420615956</v>
+        <v>0.56764427625354796</v>
       </c>
       <c r="R665">
         <v>648</v>
@@ -40479,10 +40481,10 @@
         <v>61</v>
       </c>
       <c r="D666">
-        <v>0.37121018384337801</v>
+        <v>0.58974358974358998</v>
       </c>
       <c r="E666">
-        <v>0.62878981615662199</v>
+        <v>0.41025641025641002</v>
       </c>
       <c r="F666">
         <v>88608</v>
@@ -40518,7 +40520,7 @@
         <v>0.67900000000000005</v>
       </c>
       <c r="Q666">
-        <v>0.53626801874294505</v>
+        <v>0.64754075283651003</v>
       </c>
       <c r="R666">
         <v>329</v>
@@ -40538,10 +40540,10 @@
         <v>61</v>
       </c>
       <c r="D667">
-        <v>0.46451657321205903</v>
+        <v>0.86666666666666703</v>
       </c>
       <c r="E667">
-        <v>0.53548342678794103</v>
+        <v>0.133333333333333</v>
       </c>
       <c r="F667">
         <v>56052</v>
@@ -40577,7 +40579,7 @@
         <v>0.68200000000000005</v>
       </c>
       <c r="Q667">
-        <v>0.59361883072370003</v>
+        <v>0.73157006190208196</v>
       </c>
       <c r="R667">
         <v>392</v>
@@ -40597,10 +40599,10 @@
         <v>61</v>
       </c>
       <c r="D668">
-        <v>0.45029642888035698</v>
+        <v>0.81818181818181801</v>
       </c>
       <c r="E668">
-        <v>0.54970357111964296</v>
+        <v>0.18181818181818199</v>
       </c>
       <c r="F668">
         <v>75194</v>
@@ -40636,7 +40638,7 @@
         <v>0.79200000000000004</v>
       </c>
       <c r="Q668">
-        <v>0.68403292061940801</v>
+        <v>0.79730687455705196</v>
       </c>
       <c r="R668">
         <v>321</v>
@@ -40656,10 +40658,10 @@
         <v>61</v>
       </c>
       <c r="D669">
-        <v>0.39462778101462298</v>
+        <v>0.65048543689320404</v>
       </c>
       <c r="E669">
-        <v>0.60537221898537696</v>
+        <v>0.34951456310679602</v>
       </c>
       <c r="F669">
         <v>94208</v>
@@ -40695,7 +40697,7 @@
         <v>0.878</v>
       </c>
       <c r="Q669">
-        <v>0.76385319473064295</v>
+        <v>0.84206822009400994</v>
       </c>
       <c r="R669">
         <v>240</v>
@@ -40715,10 +40717,10 @@
         <v>61</v>
       </c>
       <c r="D670">
-        <v>0.282951520984428</v>
+        <v>0.39436619718309901</v>
       </c>
       <c r="E670">
-        <v>0.717048479015572</v>
+        <v>0.60563380281690105</v>
       </c>
       <c r="F670">
         <v>92210</v>
@@ -40754,7 +40756,7 @@
         <v>0.75700000000000001</v>
       </c>
       <c r="Q670">
-        <v>0.53798023143810902</v>
+        <v>0.61874350871765404</v>
       </c>
       <c r="R670">
         <v>145</v>
@@ -40951,10 +40953,10 @@
         <v>61</v>
       </c>
       <c r="D674">
-        <v>0.28663042416745299</v>
+        <v>0.40151577334537197</v>
       </c>
       <c r="E674">
-        <v>0.71336957583254701</v>
+        <v>0.59848422665462797</v>
       </c>
       <c r="F674">
         <v>109647</v>
@@ -41010,10 +41012,10 @@
         <v>61</v>
       </c>
       <c r="D675">
-        <v>0.28663042416745299</v>
+        <v>0.40151577334537197</v>
       </c>
       <c r="E675">
-        <v>0.71336957583254701</v>
+        <v>0.59848422665462797</v>
       </c>
       <c r="F675">
         <v>109647</v>
@@ -41049,7 +41051,7 @@
         <v>0.96899999999999997</v>
       </c>
       <c r="Q675">
-        <v>0.90240229637556102</v>
+        <v>0.928326313372979</v>
       </c>
       <c r="R675" t="s">
         <v>10</v>
@@ -41069,10 +41071,10 @@
         <v>61</v>
       </c>
       <c r="D676">
-        <v>0.20580062190399301</v>
+        <v>0.25905499835909401</v>
       </c>
       <c r="E676">
-        <v>0.79419937809600705</v>
+        <v>0.74094500164090604</v>
       </c>
       <c r="F676">
         <v>124931</v>
@@ -41128,10 +41130,10 @@
         <v>61</v>
       </c>
       <c r="D677">
-        <v>0.20580062190399301</v>
+        <v>0.25905499835909401</v>
       </c>
       <c r="E677">
-        <v>0.79419937809600705</v>
+        <v>0.74094500164090604</v>
       </c>
       <c r="F677">
         <v>124931</v>
@@ -41167,7 +41169,7 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="Q677">
-        <v>0.89168140105619198</v>
+        <v>0.91198887488543401</v>
       </c>
       <c r="R677" t="s">
         <v>10</v>
@@ -41187,10 +41189,10 @@
         <v>61</v>
       </c>
       <c r="D678">
-        <v>0.36162993950820999</v>
+        <v>0.56581060006606798</v>
       </c>
       <c r="E678">
-        <v>0.63837006049179001</v>
+        <v>0.43418939993393202</v>
       </c>
       <c r="F678">
         <v>130169</v>
@@ -41246,10 +41248,10 @@
         <v>61</v>
       </c>
       <c r="D679">
-        <v>0.36162993950820999</v>
+        <v>0.56581060006606798</v>
       </c>
       <c r="E679">
-        <v>0.63837006049179001</v>
+        <v>0.43418939993393202</v>
       </c>
       <c r="F679">
         <v>130169</v>
@@ -41285,7 +41287,7 @@
         <v>0.95</v>
       </c>
       <c r="Q679">
-        <v>0.87853167323121095</v>
+        <v>0.91880620438388705</v>
       </c>
       <c r="R679" t="s">
         <v>10</v>
@@ -41305,10 +41307,10 @@
         <v>61</v>
       </c>
       <c r="D680">
-        <v>0.36253296387772299</v>
+        <v>0.56802299171878801</v>
       </c>
       <c r="E680">
-        <v>0.63746703612227695</v>
+        <v>0.43197700828121199</v>
       </c>
       <c r="F680">
         <v>114476</v>
@@ -41364,10 +41366,10 @@
         <v>61</v>
       </c>
       <c r="D681">
-        <v>0.36253296387772299</v>
+        <v>0.56802299171878801</v>
       </c>
       <c r="E681">
-        <v>0.63746703612227695</v>
+        <v>0.43197700828121199</v>
       </c>
       <c r="F681">
         <v>114476</v>
@@ -41403,7 +41405,7 @@
         <v>0.95799999999999996</v>
       </c>
       <c r="Q681">
-        <v>0.89617656964861003</v>
+        <v>0.93115013602739505</v>
       </c>
       <c r="R681" t="s">
         <v>10</v>
@@ -41423,10 +41425,10 @@
         <v>61</v>
       </c>
       <c r="D682">
-        <v>0.35846624156618101</v>
+        <v>0.55803920154787201</v>
       </c>
       <c r="E682">
-        <v>0.64153375843381899</v>
+        <v>0.44196079845212799</v>
       </c>
       <c r="F682">
         <v>83211</v>
@@ -41482,10 +41484,10 @@
         <v>61</v>
       </c>
       <c r="D683">
-        <v>0.35846624156618101</v>
+        <v>0.55803920154787201</v>
       </c>
       <c r="E683">
-        <v>0.64153375843381899</v>
+        <v>0.44196079845212799</v>
       </c>
       <c r="F683">
         <v>83211</v>
@@ -41521,7 +41523,7 @@
         <v>0.95699999999999996</v>
       </c>
       <c r="Q683">
-        <v>0.89289261325622205</v>
+        <v>0.92845724556857401</v>
       </c>
       <c r="R683" t="s">
         <v>10</v>
@@ -41541,10 +41543,10 @@
         <v>61</v>
       </c>
       <c r="D684">
-        <v>0.33398679947924598</v>
+        <v>0.50123249236081902</v>
       </c>
       <c r="E684">
-        <v>0.66601320052075397</v>
+        <v>0.49876750763918098</v>
       </c>
       <c r="F684">
         <v>88033</v>
@@ -41600,10 +41602,10 @@
         <v>61</v>
       </c>
       <c r="D685">
-        <v>0.33398679947924598</v>
+        <v>0.50123249236081902</v>
       </c>
       <c r="E685">
-        <v>0.66601320052075397</v>
+        <v>0.49876750763918098</v>
       </c>
       <c r="F685">
         <v>88033</v>
@@ -41639,7 +41641,7 @@
         <v>0.96899999999999997</v>
       </c>
       <c r="Q685">
-        <v>0.91506542142282898</v>
+        <v>0.94175477738592495</v>
       </c>
       <c r="R685" t="s">
         <v>10</v>
@@ -41659,10 +41661,10 @@
         <v>61</v>
       </c>
       <c r="D686">
-        <v>0.22695361281681301</v>
+        <v>0.293463073434794</v>
       </c>
       <c r="E686">
-        <v>0.77304638718318697</v>
+        <v>0.70653692656520595</v>
       </c>
       <c r="F686">
         <v>119521</v>
@@ -41718,10 +41720,10 @@
         <v>61</v>
       </c>
       <c r="D687">
-        <v>0.22695361281681301</v>
+        <v>0.293463073434794</v>
       </c>
       <c r="E687">
-        <v>0.77304638718318697</v>
+        <v>0.70653692656520595</v>
       </c>
       <c r="F687">
         <v>119521</v>
@@ -41757,7 +41759,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="Q687">
-        <v>0.89017610030841798</v>
+        <v>0.91289823835495798</v>
       </c>
       <c r="R687" t="s">
         <v>10</v>
@@ -41777,10 +41779,10 @@
         <v>61</v>
       </c>
       <c r="D688">
-        <v>0.34397588914771499</v>
+        <v>1</v>
       </c>
       <c r="E688">
-        <v>0.65602411085228496</v>
+        <v>0</v>
       </c>
       <c r="F688">
         <v>109418</v>
@@ -41836,10 +41838,10 @@
         <v>61</v>
       </c>
       <c r="D689">
-        <v>0.34397588914771499</v>
+        <v>1</v>
       </c>
       <c r="E689">
-        <v>0.65602411085228496</v>
+        <v>0</v>
       </c>
       <c r="F689">
         <v>109418</v>
@@ -41875,7 +41877,7 @@
         <v>0.98</v>
       </c>
       <c r="Q689">
-        <v>0.94505130533005399</v>
+        <v>0.98039215686274495</v>
       </c>
       <c r="R689" t="s">
         <v>10</v>
@@ -41895,10 +41897,10 @@
         <v>61</v>
       </c>
       <c r="D690">
-        <v>0.29568883829486797</v>
+        <v>1</v>
       </c>
       <c r="E690">
-        <v>0.70431116170513197</v>
+        <v>0</v>
       </c>
       <c r="F690">
         <v>110850</v>
@@ -41954,10 +41956,10 @@
         <v>61</v>
       </c>
       <c r="D691">
-        <v>0.29568883829486797</v>
+        <v>1</v>
       </c>
       <c r="E691">
-        <v>0.70431116170513197</v>
+        <v>0</v>
       </c>
       <c r="F691">
         <v>110850</v>
@@ -41993,7 +41995,7 @@
         <v>0.93600000000000005</v>
       </c>
       <c r="Q691">
-        <v>0.82206842919175205</v>
+        <v>0.93984962406015005</v>
       </c>
       <c r="R691" t="s">
         <v>10</v>
@@ -42013,10 +42015,10 @@
         <v>61</v>
       </c>
       <c r="D692">
-        <v>0.26534690818620699</v>
+        <v>0.36087613712003602</v>
       </c>
       <c r="E692">
-        <v>0.73465309181379301</v>
+        <v>0.63912386287996403</v>
       </c>
       <c r="F692">
         <v>144224</v>
@@ -42072,10 +42074,10 @@
         <v>61</v>
       </c>
       <c r="D693">
-        <v>0.26534690818620699</v>
+        <v>0.36087613712003602</v>
       </c>
       <c r="E693">
-        <v>0.73465309181379301</v>
+        <v>0.63912386287996403</v>
       </c>
       <c r="F693">
         <v>144224</v>
@@ -42111,7 +42113,7 @@
         <v>0.99</v>
       </c>
       <c r="Q693">
-        <v>0.96368217799911704</v>
+        <v>0.973036820115597</v>
       </c>
       <c r="R693" t="s">
         <v>10</v>
@@ -42131,10 +42133,10 @@
         <v>61</v>
       </c>
       <c r="D694">
-        <v>0.254171884867752</v>
+        <v>1</v>
       </c>
       <c r="E694">
-        <v>0.745828115132248</v>
+        <v>0</v>
       </c>
       <c r="F694">
         <v>139464</v>
@@ -42190,10 +42192,10 @@
         <v>61</v>
       </c>
       <c r="D695">
-        <v>0.254171884867752</v>
+        <v>1</v>
       </c>
       <c r="E695">
-        <v>0.745828115132248</v>
+        <v>0</v>
       </c>
       <c r="F695">
         <v>139464</v>
@@ -42229,7 +42231,7 @@
         <v>0.97299999999999998</v>
       </c>
       <c r="Q695">
-        <v>0.90397332929393204</v>
+        <v>0.97370983446932802</v>
       </c>
       <c r="R695" t="s">
         <v>10</v>
@@ -42249,10 +42251,10 @@
         <v>61</v>
       </c>
       <c r="D696">
-        <v>0.25019317805497299</v>
+        <v>0.333522179629616</v>
       </c>
       <c r="E696">
-        <v>0.74980682194502701</v>
+        <v>0.66647782037038406</v>
       </c>
       <c r="F696">
         <v>135913</v>
@@ -42308,10 +42310,10 @@
         <v>61</v>
       </c>
       <c r="D697">
-        <v>0.25019317805497299</v>
+        <v>0.333522179629616</v>
       </c>
       <c r="E697">
-        <v>0.74980682194502701</v>
+        <v>0.66647782037038406</v>
       </c>
       <c r="F697">
         <v>135913</v>
@@ -42347,7 +42349,7 @@
         <v>0.98099999999999998</v>
       </c>
       <c r="Q697">
-        <v>0.92941871656153197</v>
+        <v>0.94610268204978598</v>
       </c>
       <c r="R697" t="s">
         <v>10</v>
@@ -42544,10 +42546,10 @@
         <v>61</v>
       </c>
       <c r="D701">
-        <v>0.122624885519192</v>
+        <v>0.139718120096161</v>
       </c>
       <c r="E701">
-        <v>0.87737511448080796</v>
+        <v>0.86028187990383898</v>
       </c>
       <c r="F701">
         <v>1362708</v>
@@ -42603,10 +42605,10 @@
         <v>61</v>
       </c>
       <c r="D702">
-        <v>4.2596153351649301E-3</v>
+        <v>4.2777735113338298E-3</v>
       </c>
       <c r="E702">
-        <v>0.99574038466483505</v>
+        <v>0.99572222648866604</v>
       </c>
       <c r="F702">
         <v>1207574</v>
@@ -42642,7 +42644,7 @@
         <v>0.90100000000000002</v>
       </c>
       <c r="Q702">
-        <v>4.1251512717134099E-2</v>
+        <v>4.14200787438972E-2</v>
       </c>
       <c r="R702">
         <v>503</v>
@@ -42662,10 +42664,10 @@
         <v>61</v>
       </c>
       <c r="D703">
-        <v>6.5386673048838995E-2</v>
+        <v>6.9942721267759897E-2</v>
       </c>
       <c r="E703">
-        <v>0.93461332695116095</v>
+        <v>0.93005727873223998</v>
       </c>
       <c r="F703">
         <v>851703</v>
@@ -42701,7 +42703,7 @@
         <v>0.88</v>
       </c>
       <c r="Q703">
-        <v>0.35270428005152898</v>
+        <v>0.36823059499691202</v>
       </c>
       <c r="R703">
         <v>556</v>
@@ -42721,10 +42723,10 @@
         <v>61</v>
       </c>
       <c r="D704">
-        <v>5.8226524653898201E-2</v>
+        <v>6.18185115204661E-2</v>
       </c>
       <c r="E704">
-        <v>0.94177347534610201</v>
+        <v>0.93818148847953398</v>
       </c>
       <c r="F704">
         <v>621894</v>
@@ -42760,7 +42762,7 @@
         <v>0.94099999999999995</v>
       </c>
       <c r="Q704">
-        <v>0.49670093714547398</v>
+        <v>0.51166423706514796</v>
       </c>
       <c r="R704">
         <v>728</v>
@@ -42780,10 +42782,10 @@
         <v>61</v>
       </c>
       <c r="D705">
-        <v>4.82597848082661E-2</v>
+        <v>5.0699547383616803E-2</v>
       </c>
       <c r="E705">
-        <v>0.95174021519173402</v>
+        <v>0.94930045261638296</v>
       </c>
       <c r="F705">
         <v>1119000</v>
@@ -42819,7 +42821,7 @@
         <v>0.73399999999999999</v>
       </c>
       <c r="Q705">
-        <v>0.15356653043503499</v>
+        <v>0.16008721137262799</v>
       </c>
       <c r="R705">
         <v>719</v>
@@ -42839,10 +42841,10 @@
         <v>61</v>
       </c>
       <c r="D706">
-        <v>1.2763607965536401E-2</v>
+        <v>1.2927945311207899E-2</v>
       </c>
       <c r="E706">
-        <v>0.98723639203446401</v>
+        <v>0.987072054688792</v>
       </c>
       <c r="F706">
         <v>1067000</v>
@@ -42878,7 +42880,7 @@
         <v>0.41899999999999998</v>
       </c>
       <c r="Q706">
-        <v>2.1496110226878799E-2</v>
+        <v>2.1766858106725202E-2</v>
       </c>
       <c r="R706">
         <v>292</v>
@@ -42898,10 +42900,10 @@
         <v>61</v>
       </c>
       <c r="D707">
-        <v>5.4782947431533096E-3</v>
+        <v>5.5083362340181703E-3</v>
       </c>
       <c r="E707">
-        <v>0.99452170525684702</v>
+        <v>0.99449166376598197</v>
       </c>
       <c r="F707">
         <v>1016015</v>
@@ -42937,7 +42939,7 @@
         <v>0.68</v>
       </c>
       <c r="Q707">
-        <v>1.6831520969705301E-2</v>
+        <v>1.6922258574840501E-2</v>
       </c>
       <c r="R707">
         <v>365</v>
@@ -42957,10 +42959,10 @@
         <v>61</v>
       </c>
       <c r="D708">
-        <v>5.2424691430621303E-3</v>
+        <v>5.2700033326865403E-3</v>
       </c>
       <c r="E708">
-        <v>0.99475753085693797</v>
+        <v>0.99472999666731299</v>
       </c>
       <c r="F708">
         <v>1007734</v>
@@ -42996,7 +42998,7 @@
         <v>0.70899999999999996</v>
       </c>
       <c r="Q708">
-        <v>1.7696548230329599E-2</v>
+        <v>1.77878397185177E-2</v>
       </c>
       <c r="R708">
         <v>236</v>
@@ -43016,10 +43018,10 @@
         <v>61</v>
       </c>
       <c r="D709">
-        <v>4.6646909330140098E-3</v>
+        <v>4.68646016588795E-3</v>
       </c>
       <c r="E709">
-        <v>0.99533530906698597</v>
+        <v>0.99531353983411197</v>
       </c>
       <c r="F709">
         <v>1068770</v>
@@ -43055,7 +43057,7 @@
         <v>0.65100000000000002</v>
       </c>
       <c r="Q709">
-        <v>1.3189586217125401E-2</v>
+        <v>1.3250323927271299E-2</v>
       </c>
       <c r="R709">
         <v>271</v>
@@ -43075,10 +43077,10 @@
         <v>61</v>
       </c>
       <c r="D710">
-        <v>2.1714366815745499E-3</v>
+        <v>2.1761429214100401E-3</v>
       </c>
       <c r="E710">
-        <v>0.99782856331842495</v>
+        <v>0.99782385707859</v>
       </c>
       <c r="F710">
         <v>1135883</v>
@@ -43114,7 +43116,7 @@
         <v>0.83199999999999996</v>
       </c>
       <c r="Q710">
-        <v>1.27602888235453E-2</v>
+        <v>1.2787591045679199E-2</v>
       </c>
       <c r="R710">
         <v>124</v>
@@ -44963,10 +44965,10 @@
         <v>61</v>
       </c>
       <c r="D742">
-        <v>0.36061127627392697</v>
+        <v>0.56367193869232002</v>
       </c>
       <c r="E742">
-        <v>0.63938872372607303</v>
+        <v>0.43632806130767998</v>
       </c>
       <c r="F742">
         <v>81823</v>
@@ -45022,10 +45024,10 @@
         <v>61</v>
       </c>
       <c r="D743">
-        <v>0.23304474505723199</v>
+        <v>0.30371198107936598</v>
       </c>
       <c r="E743">
-        <v>0.76695525494276795</v>
+        <v>0.69628801892063397</v>
       </c>
       <c r="F743">
         <v>184349</v>
@@ -45081,10 +45083,10 @@
         <v>61</v>
       </c>
       <c r="D744">
-        <v>0.15602256186317301</v>
+        <v>0.18480756637571599</v>
       </c>
       <c r="E744">
-        <v>0.84397743813682702</v>
+        <v>0.81519243362428395</v>
       </c>
       <c r="F744">
         <v>120639</v>
@@ -45140,10 +45142,10 @@
         <v>61</v>
       </c>
       <c r="D745">
-        <v>0.27074123184863702</v>
+        <v>0.37090511540318499</v>
       </c>
       <c r="E745">
-        <v>0.72925876815136303</v>
+        <v>0.62909488459681495</v>
       </c>
       <c r="F745">
         <v>190794</v>
@@ -45199,10 +45201,10 @@
         <v>61</v>
       </c>
       <c r="D746">
-        <v>0.288178740230977</v>
+        <v>0.40448541584783398</v>
       </c>
       <c r="E746">
-        <v>0.711821259769023</v>
+        <v>0.59551458415216596</v>
       </c>
       <c r="F746">
         <v>167922</v>
@@ -45258,10 +45260,10 @@
         <v>61</v>
       </c>
       <c r="D747">
-        <v>0.24808232883891601</v>
+        <v>0.32972201274516</v>
       </c>
       <c r="E747">
-        <v>0.75191767116108399</v>
+        <v>0.67027798725484</v>
       </c>
       <c r="F747">
         <v>173713</v>
@@ -45317,10 +45319,10 @@
         <v>61</v>
       </c>
       <c r="D748">
-        <v>0.24951407971965001</v>
+        <v>0.33225384885092302</v>
       </c>
       <c r="E748">
-        <v>0.75048592028034999</v>
+        <v>0.66774615114907698</v>
       </c>
       <c r="F748">
         <v>156865</v>
@@ -45376,10 +45378,10 @@
         <v>61</v>
       </c>
       <c r="D749">
-        <v>0.22684796569544599</v>
+        <v>0.29323023223891898</v>
       </c>
       <c r="E749">
-        <v>0.77315203430455404</v>
+        <v>0.70676976776108102</v>
       </c>
       <c r="F749">
         <v>152989</v>
@@ -45435,10 +45437,10 @@
         <v>61</v>
       </c>
       <c r="D750">
-        <v>0.25858136198079501</v>
+        <v>0.34855810954895999</v>
       </c>
       <c r="E750">
-        <v>0.74141863801920505</v>
+        <v>0.65144189045103995</v>
       </c>
       <c r="F750">
         <v>161316</v>
@@ -45494,10 +45496,10 @@
         <v>61</v>
       </c>
       <c r="D751">
-        <v>0.26250261370764699</v>
+        <v>0.35572652626262002</v>
       </c>
       <c r="E751">
-        <v>0.73749738629235395</v>
+        <v>0.64427347373737998</v>
       </c>
       <c r="F751">
         <v>162341</v>
@@ -45553,10 +45555,10 @@
         <v>61</v>
       </c>
       <c r="D752">
-        <v>0.27606144850359599</v>
+        <v>0.38109452138713001</v>
       </c>
       <c r="E752">
-        <v>0.72393855149640396</v>
+        <v>0.61890547861287004</v>
       </c>
       <c r="F752">
         <v>166502</v>
@@ -45612,10 +45614,10 @@
         <v>61</v>
       </c>
       <c r="D753">
-        <v>0.24741063168286001</v>
+        <v>0.34865129679257201</v>
       </c>
       <c r="E753">
-        <v>0.75258936831713996</v>
+        <v>0.65134870320742799</v>
       </c>
       <c r="F753">
         <v>154111</v>
@@ -47204,11 +47206,11 @@
       <c r="C780" t="s">
         <v>61</v>
       </c>
-      <c r="D780">
-        <v>0</v>
-      </c>
-      <c r="E780">
-        <v>1</v>
+      <c r="D780" t="s">
+        <v>10</v>
+      </c>
+      <c r="E780" t="s">
+        <v>10</v>
       </c>
       <c r="F780">
         <v>39588</v>
@@ -48385,10 +48387,10 @@
         <v>61</v>
       </c>
       <c r="D800">
-        <v>0.50084718266700301</v>
+        <v>1</v>
       </c>
       <c r="E800">
-        <v>0.49915281733299699</v>
+        <v>0</v>
       </c>
       <c r="F800">
         <v>41679</v>
@@ -48444,10 +48446,10 @@
         <v>61</v>
       </c>
       <c r="D801">
-        <v>0.50076935586774596</v>
+        <v>1</v>
       </c>
       <c r="E801">
-        <v>0.49923064413225399</v>
+        <v>0</v>
       </c>
       <c r="F801">
         <v>40030</v>
@@ -48503,10 +48505,10 @@
         <v>61</v>
       </c>
       <c r="D802">
-        <v>0.45580955431141801</v>
+        <v>0.83673469387755095</v>
       </c>
       <c r="E802">
-        <v>0.54419044568858199</v>
+        <v>0.16326530612244899</v>
       </c>
       <c r="F802">
         <v>40058</v>
@@ -48542,7 +48544,7 @@
         <v>0.66100000000000003</v>
       </c>
       <c r="Q802">
-        <v>0.57348273160393504</v>
+        <v>0.71166964642168995</v>
       </c>
       <c r="R802">
         <v>363</v>
@@ -48562,10 +48564,10 @@
         <v>61</v>
       </c>
       <c r="D803">
-        <v>0.50032243001045096</v>
+        <v>1</v>
       </c>
       <c r="E803">
-        <v>0.49967756998954899</v>
+        <v>0</v>
       </c>
       <c r="F803">
         <v>45000</v>
@@ -48601,7 +48603,7 @@
         <v>0.71</v>
       </c>
       <c r="Q803">
-        <v>0.63306115455161105</v>
+        <v>0.775193798449612</v>
       </c>
       <c r="R803">
         <v>364</v>
@@ -48621,10 +48623,10 @@
         <v>61</v>
       </c>
       <c r="D804">
-        <v>0.43053415782031501</v>
+        <v>0.75555555555555598</v>
       </c>
       <c r="E804">
-        <v>0.56946584217968499</v>
+        <v>0.24444444444444399</v>
       </c>
       <c r="F804">
         <v>54000</v>
@@ -48660,7 +48662,7 @@
         <v>0.871</v>
       </c>
       <c r="Q804">
-        <v>0.76945107247335198</v>
+        <v>0.85416404974249505</v>
       </c>
       <c r="R804">
         <v>155</v>
@@ -48680,10 +48682,10 @@
         <v>61</v>
       </c>
       <c r="D805">
-        <v>0.48564975600064098</v>
+        <v>0.94230769230769196</v>
       </c>
       <c r="E805">
-        <v>0.51435024399935902</v>
+        <v>5.7692307692307702E-2</v>
       </c>
       <c r="F805">
         <v>48886</v>
@@ -48719,7 +48721,7 @@
         <v>0.91200000000000003</v>
       </c>
       <c r="Q805">
-        <v>0.84659629141391701</v>
+        <v>0.91458862177094202</v>
       </c>
       <c r="R805">
         <v>166</v>
@@ -48739,10 +48741,10 @@
         <v>61</v>
       </c>
       <c r="D806">
-        <v>0.50050685123042504</v>
+        <v>1</v>
       </c>
       <c r="E806">
-        <v>0.49949314876957501</v>
+        <v>0</v>
       </c>
       <c r="F806">
         <v>57274</v>
@@ -48778,7 +48780,7 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="Q806">
-        <v>0.709428760837015</v>
+        <v>0.829875518672199</v>
       </c>
       <c r="R806">
         <v>194</v>
@@ -48798,10 +48800,10 @@
         <v>61</v>
       </c>
       <c r="D807">
-        <v>0.32274372793832201</v>
+        <v>0.476190476190476</v>
       </c>
       <c r="E807">
-        <v>0.67725627206167804</v>
+        <v>0.52380952380952395</v>
       </c>
       <c r="F807">
         <v>53625</v>
@@ -48837,7 +48839,7 @@
         <v>0.69299999999999995</v>
       </c>
       <c r="Q807">
-        <v>0.51250010697991699</v>
+        <v>0.60801361950507704</v>
       </c>
       <c r="R807">
         <v>185</v>
@@ -48857,10 +48859,10 @@
         <v>61</v>
       </c>
       <c r="D808">
-        <v>0.23924736531714599</v>
+        <v>0.314285714285714</v>
       </c>
       <c r="E808">
-        <v>0.76075263468285403</v>
+        <v>0.68571428571428605</v>
       </c>
       <c r="F808">
         <v>51374</v>
@@ -48916,10 +48918,10 @@
         <v>61</v>
       </c>
       <c r="D809">
-        <v>0.215769260365585</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="E809">
-        <v>0.78423073963441503</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="F809">
         <v>44864</v>
@@ -49211,10 +49213,10 @@
         <v>61</v>
       </c>
       <c r="D814">
-        <v>0.50047589747534005</v>
+        <v>1</v>
       </c>
       <c r="E814">
-        <v>0.49952410252466001</v>
+        <v>0</v>
       </c>
       <c r="F814">
         <v>104113</v>
@@ -49270,10 +49272,10 @@
         <v>61</v>
       </c>
       <c r="D815">
-        <v>9.3348367616190794E-2</v>
+        <v>0.10294117647058799</v>
       </c>
       <c r="E815">
-        <v>0.90665163238380897</v>
+        <v>0.89705882352941202</v>
       </c>
       <c r="F815">
         <v>118220</v>
@@ -49309,7 +49311,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="Q815">
-        <v>9.3502799868430395E-2</v>
+        <v>0.1021301429822</v>
       </c>
       <c r="R815">
         <v>24</v>
@@ -49329,10 +49331,10 @@
         <v>61</v>
       </c>
       <c r="D816">
-        <v>0.32323045818844598</v>
+        <v>0.47727272727272702</v>
       </c>
       <c r="E816">
-        <v>0.67676954181155402</v>
+        <v>0.52272727272727304</v>
       </c>
       <c r="F816">
         <v>119708</v>
@@ -49368,7 +49370,7 @@
         <v>0.33600000000000002</v>
       </c>
       <c r="Q816">
-        <v>0.32741135112622999</v>
+        <v>0.41819340449259201</v>
       </c>
       <c r="R816">
         <v>151</v>
@@ -49388,10 +49390,10 @@
         <v>61</v>
       </c>
       <c r="D817">
-        <v>0.37827849368101002</v>
+        <v>0.60784313725490202</v>
       </c>
       <c r="E817">
-        <v>0.62172150631899004</v>
+        <v>0.39215686274509798</v>
       </c>
       <c r="F817">
         <v>127000</v>
@@ -49427,7 +49429,7 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="Q817">
-        <v>0.34039936508444102</v>
+        <v>0.453329043768188</v>
       </c>
       <c r="R817">
         <v>120</v>
@@ -49447,10 +49449,10 @@
         <v>61</v>
       </c>
       <c r="D818">
-        <v>0.464395419777136</v>
+        <v>0.86585365853658502</v>
       </c>
       <c r="E818">
-        <v>0.53560458022286395</v>
+        <v>0.134146341463415</v>
       </c>
       <c r="F818">
         <v>103000</v>
@@ -49486,7 +49488,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="Q818">
-        <v>0.58093330070192895</v>
+        <v>0.72103178633086196</v>
       </c>
       <c r="R818">
         <v>216</v>
@@ -49506,10 +49508,10 @@
         <v>61</v>
       </c>
       <c r="D819">
-        <v>0.33625000017786599</v>
+        <v>0.50602409638554202</v>
       </c>
       <c r="E819">
-        <v>0.66374999982213401</v>
+        <v>0.49397590361445798</v>
       </c>
       <c r="F819">
         <v>112528</v>
@@ -49545,7 +49547,7 @@
         <v>0.68300000000000005</v>
       </c>
       <c r="Q819">
-        <v>0.51473402232883603</v>
+        <v>0.61483509244484802</v>
       </c>
       <c r="R819">
         <v>400</v>
@@ -49565,10 +49567,10 @@
         <v>61</v>
       </c>
       <c r="D820">
-        <v>0.26974129791527202</v>
+        <v>0.36904761904761901</v>
       </c>
       <c r="E820">
-        <v>0.73025870208472798</v>
+        <v>0.63095238095238104</v>
       </c>
       <c r="F820">
         <v>104064</v>
@@ -49604,7 +49606,7 @@
         <v>0.84299999999999997</v>
       </c>
       <c r="Q820">
-        <v>0.63209560272938103</v>
+        <v>0.70154793156513096</v>
       </c>
       <c r="R820">
         <v>118</v>
@@ -49624,10 +49626,10 @@
         <v>61</v>
       </c>
       <c r="D821">
-        <v>0.42602924904251199</v>
+        <v>0.74074074074074103</v>
       </c>
       <c r="E821">
-        <v>0.57397075095748795</v>
+        <v>0.25925925925925902</v>
       </c>
       <c r="F821">
         <v>118105</v>
@@ -49663,7 +49665,7 @@
         <v>0.65800000000000003</v>
       </c>
       <c r="Q821">
-        <v>0.55470445894298304</v>
+        <v>0.68413491140452898</v>
       </c>
       <c r="R821">
         <v>513</v>
@@ -49683,10 +49685,10 @@
         <v>61</v>
       </c>
       <c r="D822">
-        <v>0.50031696279209004</v>
+        <v>1</v>
       </c>
       <c r="E822">
-        <v>0.49968303720791002</v>
+        <v>0</v>
       </c>
       <c r="F822">
         <v>113650</v>
@@ -49742,10 +49744,10 @@
         <v>61</v>
       </c>
       <c r="D823">
-        <v>0.250090130064616</v>
+        <v>0.33333333333333298</v>
       </c>
       <c r="E823">
-        <v>0.749909869935384</v>
+        <v>0.66666666666666696</v>
       </c>
       <c r="F823">
         <v>108216</v>
@@ -56466,7 +56468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -56485,7 +56487,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>83</v>
       </c>
       <c r="B2" t="s">

</xml_diff>